<commit_message>
Adds publications until 2018
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -8,19 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/vem2004-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C618908F-4093-E94D-A406-B18C184B199D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144A3615-122A-AE47-BA77-2AD62A99FC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="23260" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId2"/>
-    <sheet name="vem2017" sheetId="3" r:id="rId3"/>
-    <sheet name="vem2018" sheetId="4" r:id="rId4"/>
-    <sheet name="vem2019" sheetId="5" r:id="rId5"/>
-    <sheet name="vem2020" sheetId="6" r:id="rId6"/>
-    <sheet name="vem2021" sheetId="7" r:id="rId7"/>
-    <sheet name="vem2022" sheetId="8" r:id="rId8"/>
+    <sheet name="publications" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="488">
   <si>
     <t>title</t>
   </si>
@@ -1222,6 +1215,288 @@
   </si>
   <si>
     <t>Laerte Xavier; Aline Brito; André Hora; Marco Tulio Valente </t>
+  </si>
+  <si>
+    <t>Caracterização do Papel Desempenhado por Desenvolvedores Responsáveis pelo Truck Factor de Projetos de Software</t>
+  </si>
+  <si>
+    <t>Como Pesquisadores Usam o Dataset GHTorrent?</t>
+  </si>
+  <si>
+    <t>Uma Análise Preliminar da Hiperespecialização no Contexto de Crowdsourcing na Plataforma Topcoder</t>
+  </si>
+  <si>
+    <t>Who Drive Company-Owned OSS Projects: Employees or Volunteers?</t>
+  </si>
+  <si>
+    <t>Do Coupling Metrics Help Characterize Critical Components in Component-based SPL? An Empirical Study</t>
+  </si>
+  <si>
+    <t>Impactos de Práticas de Codificação sobre a Legibilidade: Um Estudo Preliminar</t>
+  </si>
+  <si>
+    <t>VisminerTD: Uma Ferramenta para Identificação Automática e Monitoramento Interativo de Dívida Técnica</t>
+  </si>
+  <si>
+    <t>Vulnerabilidades em Sistemas de Software Web baseados em Plug-ins: Um Estudo Exploratório do WordPress</t>
+  </si>
+  <si>
+    <t>Em Busca de uma Abordagem de Conformidade Arquitetural para Arquitetura de Microsserviços</t>
+  </si>
+  <si>
+    <t>Arquitetura de Aplicações Spring MVC: Uma Análise Baseada no Acoplamento Lógico</t>
+  </si>
+  <si>
+    <t>Uma Caracterização em Larga Escala da Arquitetura de Sistemas Docker</t>
+  </si>
+  <si>
+    <t>Usando aprendizagem de máquina para identificar anomalias de design prejudiciais à manutenibilidade: um estudo preliminar</t>
+  </si>
+  <si>
+    <t>Mineração de regras para solução de problemas relacionados à fragmentação do Android</t>
+  </si>
+  <si>
+    <t>Definição de clusters para classificação do uso de anotações em código Java</t>
+  </si>
+  <si>
+    <t>Rodrigo Magalhães Dos Santos; Marco Aurélio Gerosa </t>
+  </si>
+  <si>
+    <t>Phyllipe Lima; Eduardo Guerra; Paulo Meirelles </t>
+  </si>
+  <si>
+    <t>Thaís Mombach; Mívian Ferreira; Marco Tulio Valente; Kecia Ferreira </t>
+  </si>
+  <si>
+    <t>Hudson Borges; Jailton Coelho; Paulo Carvalho; Mariane Fernandes; Marco Tulio Valente </t>
+  </si>
+  <si>
+    <t>Anderson Bergamini de Neira; Igor Scaliante Wiese; Igor Steinmacher </t>
+  </si>
+  <si>
+    <t>Luiz Felipe Dias; Jhoylan Santos; Igor Steinmacher; Gustavo Pinto </t>
+  </si>
+  <si>
+    <t>Anderson Uchôa; Eduardo Fernandes; Ana Carla Bibiano; Alessandro Garcia </t>
+  </si>
+  <si>
+    <t>Thiago Mendes; David Gonçalves; Felipe Gomes; Renato Novais; Rodrigo Spínola; Manoel Mendonça </t>
+  </si>
+  <si>
+    <t>Oslien Mesa; Marx Viana; Elder Cirilo; Carlos Lucena </t>
+  </si>
+  <si>
+    <t>Eduardo Pereira de Sousa; Eduardo Martins Guerra; Gustavo Ansaldi Oliva; Mauricio Finavaro Aniche </t>
+  </si>
+  <si>
+    <t>Lucas Monteiro; Laerte Xavier; Marco Tulio Valente </t>
+  </si>
+  <si>
+    <t>Fabricio F Cardim; Cláudio Sant’Anna </t>
+  </si>
+  <si>
+    <t>Marcus Adriano F Pereira; Marcelo Maia </t>
+  </si>
+  <si>
+    <t>Elena A. Araujo; Elder Rodrigues Jr; Arthur F. Pinto; Ricardo Terra </t>
+  </si>
+  <si>
+    <t>UEM; UTFPR</t>
+  </si>
+  <si>
+    <t>UTFPR; UFPA</t>
+  </si>
+  <si>
+    <t>PUC-Rio</t>
+  </si>
+  <si>
+    <t>IPT-SP; NAU</t>
+  </si>
+  <si>
+    <t>PUC-Rio; UFJF; FIVJ</t>
+  </si>
+  <si>
+    <t>UFLA</t>
+  </si>
+  <si>
+    <t>INPE; Queen's University; Delft University</t>
+  </si>
+  <si>
+    <t>Caracterizando o Consumo de Energia de APIs de E/S da Linguagem Java</t>
+  </si>
+  <si>
+    <t>Um Estudo em Larga-Escala sobre Características de APIs Populares</t>
+  </si>
+  <si>
+    <t>Minerando Mensagens de Depreciação Faltantes em APIs: Um Estudo de Caso no Ecossistema Android</t>
+  </si>
+  <si>
+    <t>STF: uma abordagem Social para estimar Truck Factor no GitHub</t>
+  </si>
+  <si>
+    <t>Heurísticas para Identificação de Ambiguidade de Autores em Projetos Open Source</t>
+  </si>
+  <si>
+    <t>Monorepos: A Multivocal Literature Review</t>
+  </si>
+  <si>
+    <t>Minerando Código Comentado</t>
+  </si>
+  <si>
+    <t>Um Estudo Empírico sobre Critérios de Seleção de Repositórios GitHub</t>
+  </si>
+  <si>
+    <t>GitHub REST API vs GHTorrent vs GitHub Archive: A Comparative Study</t>
+  </si>
+  <si>
+    <t>Microservices in Practice: A Survey Study</t>
+  </si>
+  <si>
+    <t>Um Método para Detectar Similaridade entre Sistemas baseado em Decisões de Design: um Estudo Preliminar</t>
+  </si>
+  <si>
+    <t>Comparando Técnicas de Extração de Valores Limiares para Métricas: Um Estudo Preliminar com Desenvolvedores Web</t>
+  </si>
+  <si>
+    <t>Um Estudo Empírico sobre o Impacto dos Pré-processamentos e Normalizações no Cálculo do Acoplamento Conceitual</t>
+  </si>
+  <si>
+    <t>Violação de padrões de uso de APIs em sistemas configuráveis</t>
+  </si>
+  <si>
+    <t>Avaliação da Frequência de Mudanças em Dependências entre Variabilidades em Sistemas Configuráveis</t>
+  </si>
+  <si>
+    <t>VMAG 3D – An approach for supporting the comprehension of software system models using motion control in a multiuser 3D visualization environment</t>
+  </si>
+  <si>
+    <t>Development and Maintenance of Model-Oriented Software with Visualization - Exploratory and Experimental Study</t>
+  </si>
+  <si>
+    <t>Uma Análise da Produção Científica Brasileira em Conferências de Manutenção e Evolução de Software</t>
+  </si>
+  <si>
+    <t>An Infrastructure for Software Release Analysis through Provenance Graphs</t>
+  </si>
+  <si>
+    <t>Uma técnica para a quantificação do esforço de merge</t>
+  </si>
+  <si>
+    <t>Towards an automated approach for bug fix pattern detection</t>
+  </si>
+  <si>
+    <t>Explorando Como Bibliotecas Python Lançam Exceções ao Longo de sua Evolução</t>
+  </si>
+  <si>
+    <t>Identifying Confusing Code in Swift Programs</t>
+  </si>
+  <si>
+    <t>Fernando Castor</t>
+  </si>
+  <si>
+    <t>DiffMutAnalyze: Uma abordagem para auxiliar a identificação de mutantes equivalentes</t>
+  </si>
+  <si>
+    <t>Gilson Rocha; Gustavo Pinto; Fernando Castor</t>
+  </si>
+  <si>
+    <t>Caroline Lima; Pedro Henrique de Moraes; Andre Hora</t>
+  </si>
+  <si>
+    <t>Pedro Henrique de Moraes; Caroline Lima; Andre Hora</t>
+  </si>
+  <si>
+    <t>Hercules Sandim; Michele A. Brandão; Mirella M. Moro</t>
+  </si>
+  <si>
+    <t>Talita Santana Orfano; Kecia Aline Marques Ferreira; Mariza Andrade Da Silva Bigonha</t>
+  </si>
+  <si>
+    <t>Gleison Brito; Ricardo Terra; Marco Tulio Valente</t>
+  </si>
+  <si>
+    <t>Lucas Grijó; Andre Hora</t>
+  </si>
+  <si>
+    <t>Laerte Xavier; Jailton Coelho; Luciana L. Silva</t>
+  </si>
+  <si>
+    <t>Thaís Mombach; Marco Tulio Valente</t>
+  </si>
+  <si>
+    <t>Markos Viggiato; Ricardo Terra; Henrique Rocha; Marco Tulio Valente; Eduardo Figueiredo</t>
+  </si>
+  <si>
+    <t>Marcos Dósea; Claudio Sant'Anna</t>
+  </si>
+  <si>
+    <t>Raphael Lima; Marcos Dósea; Cláudio Sant'Anna</t>
+  </si>
+  <si>
+    <t>Paulo Batista Da Costa; Igor Scaliante Wiese; Reginaldo Re; Igor Steinmacher</t>
+  </si>
+  <si>
+    <t>Bruno Mecca; Diogo Boaventura; Bruno Cafeo; Elder Cirilo</t>
+  </si>
+  <si>
+    <t>Raiza Artemam de Oliveira; Bruno Gonçalves Mecca; Bruno Barbieri de Pontes Cafeo; Andre Hora</t>
+  </si>
+  <si>
+    <t>Sergio Henriques Martins Barreto Bento Antunes; Claudia Susie Camargo Rodrigues; Cláudia Maria Lima Werner</t>
+  </si>
+  <si>
+    <t>Thiago Gottardi; Rosana Braga</t>
+  </si>
+  <si>
+    <t>Klérisson Paixão; Marcelo Maia; Marco Tulio Valente</t>
+  </si>
+  <si>
+    <t>Felipe Curty; Troy Kohwalter; Vanessa Braganholo; Leonardo Murta</t>
+  </si>
+  <si>
+    <t>Tayane Moura; Leonardo Murta</t>
+  </si>
+  <si>
+    <t>Fernanda Madeiral; Thomas Durieux; Victor Sobreira; Marcelo Maia</t>
+  </si>
+  <si>
+    <t>Allan Gonçalves; Cinthia Nascimento; Eiji Adachi</t>
+  </si>
+  <si>
+    <t>Juliana Botelho; Carlos Henrique Pereira; Vinicius H. S. Durelli; Rafael S. Durelli</t>
+  </si>
+  <si>
+    <t>UFPA; UFPE</t>
+  </si>
+  <si>
+    <t>UFMG; IFMG</t>
+  </si>
+  <si>
+    <t>UFMG; UFLA; Inria</t>
+  </si>
+  <si>
+    <t>UFBA; UFS</t>
+  </si>
+  <si>
+    <t>UTFPR</t>
+  </si>
+  <si>
+    <t>UFMS; UFSJ</t>
+  </si>
+  <si>
+    <t>UFU; UFMG</t>
+  </si>
+  <si>
+    <t>UFU; Inria</t>
+  </si>
+  <si>
+    <t>UFRN</t>
+  </si>
+  <si>
+    <t>UFPE</t>
+  </si>
+  <si>
+    <t>UFLA; UFSJ</t>
   </si>
 </sst>
 </file>
@@ -3383,9 +3658,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="G182" sqref="G182"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5995,214 +6272,654 @@
         <v>2016</v>
       </c>
     </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>394</v>
+      </c>
+      <c r="B154" t="s">
+        <v>410</v>
+      </c>
+      <c r="C154" t="s">
+        <v>375</v>
+      </c>
+      <c r="D154" t="s">
+        <v>271</v>
+      </c>
+      <c r="E154">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>395</v>
+      </c>
+      <c r="B155" t="s">
+        <v>411</v>
+      </c>
+      <c r="C155" t="s">
+        <v>162</v>
+      </c>
+      <c r="D155" t="s">
+        <v>271</v>
+      </c>
+      <c r="E155">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>396</v>
+      </c>
+      <c r="B156" t="s">
+        <v>412</v>
+      </c>
+      <c r="C156" t="s">
+        <v>422</v>
+      </c>
+      <c r="D156" t="s">
+        <v>271</v>
+      </c>
+      <c r="E156">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>397</v>
+      </c>
+      <c r="B157" t="s">
+        <v>413</v>
+      </c>
+      <c r="C157" t="s">
+        <v>423</v>
+      </c>
+      <c r="D157" t="s">
+        <v>271</v>
+      </c>
+      <c r="E157">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>398</v>
+      </c>
+      <c r="B158" t="s">
+        <v>414</v>
+      </c>
+      <c r="C158" t="s">
+        <v>424</v>
+      </c>
+      <c r="D158" t="s">
+        <v>271</v>
+      </c>
+      <c r="E158">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>399</v>
+      </c>
+      <c r="B159" t="s">
+        <v>408</v>
+      </c>
+      <c r="C159" t="s">
+        <v>425</v>
+      </c>
+      <c r="D159" t="s">
+        <v>271</v>
+      </c>
+      <c r="E159">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>400</v>
+      </c>
+      <c r="B160" t="s">
+        <v>415</v>
+      </c>
+      <c r="C160" t="s">
+        <v>377</v>
+      </c>
+      <c r="D160" t="s">
+        <v>271</v>
+      </c>
+      <c r="E160">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>401</v>
+      </c>
+      <c r="B161" t="s">
+        <v>416</v>
+      </c>
+      <c r="C161" t="s">
+        <v>426</v>
+      </c>
+      <c r="D161" t="s">
+        <v>271</v>
+      </c>
+      <c r="E161">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>402</v>
+      </c>
+      <c r="B162" t="s">
+        <v>421</v>
+      </c>
+      <c r="C162" t="s">
+        <v>427</v>
+      </c>
+      <c r="D162" t="s">
+        <v>271</v>
+      </c>
+      <c r="E162">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>403</v>
+      </c>
+      <c r="B163" t="s">
+        <v>417</v>
+      </c>
+      <c r="C163" t="s">
+        <v>428</v>
+      </c>
+      <c r="D163" t="s">
+        <v>271</v>
+      </c>
+      <c r="E163">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>404</v>
+      </c>
+      <c r="B164" t="s">
+        <v>418</v>
+      </c>
+      <c r="C164" t="s">
+        <v>162</v>
+      </c>
+      <c r="D164" t="s">
+        <v>271</v>
+      </c>
+      <c r="E164">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>405</v>
+      </c>
+      <c r="B165" t="s">
+        <v>419</v>
+      </c>
+      <c r="C165" t="s">
+        <v>179</v>
+      </c>
+      <c r="D165" t="s">
+        <v>271</v>
+      </c>
+      <c r="E165">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>406</v>
+      </c>
+      <c r="B166" t="s">
+        <v>420</v>
+      </c>
+      <c r="C166" t="s">
+        <v>108</v>
+      </c>
+      <c r="D166" t="s">
+        <v>271</v>
+      </c>
+      <c r="E166">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>407</v>
+      </c>
+      <c r="B167" t="s">
+        <v>409</v>
+      </c>
+      <c r="C167" t="s">
+        <v>355</v>
+      </c>
+      <c r="D167" t="s">
+        <v>271</v>
+      </c>
+      <c r="E167">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>429</v>
+      </c>
+      <c r="B168" t="s">
+        <v>454</v>
+      </c>
+      <c r="C168" t="s">
+        <v>477</v>
+      </c>
+      <c r="D168" t="s">
+        <v>271</v>
+      </c>
+      <c r="E168">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>430</v>
+      </c>
+      <c r="B169" t="s">
+        <v>455</v>
+      </c>
+      <c r="C169" t="s">
+        <v>308</v>
+      </c>
+      <c r="D169" t="s">
+        <v>271</v>
+      </c>
+      <c r="E169">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>431</v>
+      </c>
+      <c r="B170" t="s">
+        <v>456</v>
+      </c>
+      <c r="C170" t="s">
+        <v>308</v>
+      </c>
+      <c r="D170" t="s">
+        <v>271</v>
+      </c>
+      <c r="E170">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>432</v>
+      </c>
+      <c r="B171" t="s">
+        <v>457</v>
+      </c>
+      <c r="C171" t="s">
+        <v>162</v>
+      </c>
+      <c r="D171" t="s">
+        <v>271</v>
+      </c>
+      <c r="E171">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>433</v>
+      </c>
+      <c r="B172" t="s">
+        <v>458</v>
+      </c>
+      <c r="C172" t="s">
+        <v>375</v>
+      </c>
+      <c r="D172" t="s">
+        <v>271</v>
+      </c>
+      <c r="E172">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>434</v>
+      </c>
+      <c r="B173" t="s">
+        <v>459</v>
+      </c>
+      <c r="C173" t="s">
+        <v>165</v>
+      </c>
+      <c r="D173" t="s">
+        <v>271</v>
+      </c>
+      <c r="E173">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>435</v>
+      </c>
+      <c r="B174" t="s">
+        <v>460</v>
+      </c>
+      <c r="C174" t="s">
+        <v>308</v>
+      </c>
+      <c r="D174" t="s">
+        <v>271</v>
+      </c>
+      <c r="E174">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>436</v>
+      </c>
+      <c r="B175" t="s">
+        <v>461</v>
+      </c>
+      <c r="C175" t="s">
+        <v>478</v>
+      </c>
+      <c r="D175" t="s">
+        <v>271</v>
+      </c>
+      <c r="E175">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>437</v>
+      </c>
+      <c r="B176" t="s">
+        <v>462</v>
+      </c>
+      <c r="C176" t="s">
+        <v>162</v>
+      </c>
+      <c r="D176" t="s">
+        <v>271</v>
+      </c>
+      <c r="E176">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>438</v>
+      </c>
+      <c r="B177" t="s">
+        <v>463</v>
+      </c>
+      <c r="C177" t="s">
+        <v>479</v>
+      </c>
+      <c r="D177" t="s">
+        <v>271</v>
+      </c>
+      <c r="E177">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>439</v>
+      </c>
+      <c r="B178" t="s">
+        <v>464</v>
+      </c>
+      <c r="C178" t="s">
+        <v>480</v>
+      </c>
+      <c r="D178" t="s">
+        <v>271</v>
+      </c>
+      <c r="E178">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>440</v>
+      </c>
+      <c r="B179" t="s">
+        <v>465</v>
+      </c>
+      <c r="C179" t="s">
+        <v>480</v>
+      </c>
+      <c r="D179" t="s">
+        <v>271</v>
+      </c>
+      <c r="E179">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>441</v>
+      </c>
+      <c r="B180" t="s">
+        <v>466</v>
+      </c>
+      <c r="C180" t="s">
+        <v>481</v>
+      </c>
+      <c r="D180" t="s">
+        <v>271</v>
+      </c>
+      <c r="E180">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>442</v>
+      </c>
+      <c r="B181" t="s">
+        <v>467</v>
+      </c>
+      <c r="C181" t="s">
+        <v>482</v>
+      </c>
+      <c r="D181" t="s">
+        <v>271</v>
+      </c>
+      <c r="E181">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>443</v>
+      </c>
+      <c r="B182" t="s">
+        <v>468</v>
+      </c>
+      <c r="C182" t="s">
+        <v>308</v>
+      </c>
+      <c r="D182" t="s">
+        <v>271</v>
+      </c>
+      <c r="E182">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>444</v>
+      </c>
+      <c r="B183" t="s">
+        <v>469</v>
+      </c>
+      <c r="C183" t="s">
+        <v>7</v>
+      </c>
+      <c r="D183" t="s">
+        <v>271</v>
+      </c>
+      <c r="E183">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>445</v>
+      </c>
+      <c r="B184" t="s">
+        <v>470</v>
+      </c>
+      <c r="C184" t="s">
+        <v>14</v>
+      </c>
+      <c r="D184" t="s">
+        <v>271</v>
+      </c>
+      <c r="E184">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>446</v>
+      </c>
+      <c r="B185" t="s">
+        <v>471</v>
+      </c>
+      <c r="C185" t="s">
+        <v>483</v>
+      </c>
+      <c r="D185" t="s">
+        <v>271</v>
+      </c>
+      <c r="E185">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>447</v>
+      </c>
+      <c r="B186" t="s">
+        <v>472</v>
+      </c>
+      <c r="C186" t="s">
+        <v>185</v>
+      </c>
+      <c r="D186" t="s">
+        <v>271</v>
+      </c>
+      <c r="E186">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>448</v>
+      </c>
+      <c r="B187" t="s">
+        <v>473</v>
+      </c>
+      <c r="C187" t="s">
+        <v>185</v>
+      </c>
+      <c r="D187" t="s">
+        <v>271</v>
+      </c>
+      <c r="E187">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>449</v>
+      </c>
+      <c r="B188" t="s">
+        <v>474</v>
+      </c>
+      <c r="C188" t="s">
+        <v>484</v>
+      </c>
+      <c r="D188" t="s">
+        <v>271</v>
+      </c>
+      <c r="E188">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>450</v>
+      </c>
+      <c r="B189" t="s">
+        <v>475</v>
+      </c>
+      <c r="C189" t="s">
+        <v>485</v>
+      </c>
+      <c r="D189" t="s">
+        <v>271</v>
+      </c>
+      <c r="E189">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>451</v>
+      </c>
+      <c r="B190" t="s">
+        <v>452</v>
+      </c>
+      <c r="C190" t="s">
+        <v>486</v>
+      </c>
+      <c r="D190" t="s">
+        <v>271</v>
+      </c>
+      <c r="E190">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>453</v>
+      </c>
+      <c r="B191" t="s">
+        <v>476</v>
+      </c>
+      <c r="C191" t="s">
+        <v>487</v>
+      </c>
+      <c r="D191" t="s">
+        <v>271</v>
+      </c>
+      <c r="E191">
+        <v>2018</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC8C549-9012-40B9-9736-188B64765BBB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8B6B6F-A105-47B0-BBBC-E166C3AFAF0C}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E2BD95-49B3-41F5-8C42-D8B5416CEAA5}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BE89D2-352E-47CD-85C7-31B2C140A317}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4EBF03-FA33-4D54-AA00-014254398CD5}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E02ED6-410F-45F1-A80A-1DF1269BF0F4}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506FE7DE-D5CD-45FA-9CD4-BE8F56B70BE5}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds publications from 2019 to 2021
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/vem2004-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144A3615-122A-AE47-BA77-2AD62A99FC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EA200F-4D6C-1B47-B43D-70CD5B89875D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="563">
   <si>
     <t>title</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Leonardo Murta; Hamilton Oliveira; Cristine Dantas; Luiz Gustavo Lopes; Cláudia Werner</t>
   </si>
   <si>
-    <t>COPPE/UFRJ</t>
-  </si>
-  <si>
     <t>wmswm</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Márcio Greyck Batista Dias</t>
   </si>
   <si>
-    <t>UNIGOIÁS ANHANGUERA</t>
-  </si>
-  <si>
     <t>Identificação de Padrões Arquiteturais Usando Engenharia Reversa</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Aline Vasconcelos; Cláudia Werner</t>
   </si>
   <si>
-    <t>COPPE/UFRJ; CEFET Campos</t>
-  </si>
-  <si>
     <t>Manutençäo de Sistemas OO utilizando a OA</t>
   </si>
   <si>
@@ -152,9 +143,6 @@
     <t>Natasha A.Y. do Valle; Raquel C. De Sousa; Valéria A.F. Unsonst; Nicolas Anquetil</t>
   </si>
   <si>
-    <t>Banco do Brasil – Complexo Central de Tecnologia; UCB</t>
-  </si>
-  <si>
     <t>Controle de Modificações em Software no Desenvolvimento Baseado em Componentes</t>
   </si>
   <si>
@@ -254,9 +242,6 @@
     <t>Pollyana Lima Barreto; André Villas Boas</t>
   </si>
   <si>
-    <t>SERPRO; CPQD – Telecom &amp; IT Solutions</t>
-  </si>
-  <si>
     <t>Evolucao da complexidade de tres sistemas legados</t>
   </si>
   <si>
@@ -296,9 +281,6 @@
     <t>Denis P. Pinheiro; Rodrigo G. Ribeiro; Ademir A. Oliveira; Marcelo A. Maia; Roberto S. Bigonha</t>
   </si>
   <si>
-    <t>UFMG; UFU; Google Inc.</t>
-  </si>
-  <si>
     <t>Integrated Approach for Framework-Based System Redesign</t>
   </si>
   <si>
@@ -350,9 +332,6 @@
     <t>Rodrigo P. dos Santos; Cláudia M. L. Werner; Heitor A. X. Costa; Paulo A. P. Júnior; André F. Amâncio; Antônio M. P. de Resende</t>
   </si>
   <si>
-    <t>UFLA; COPPE/UFRJ</t>
-  </si>
-  <si>
     <t>Analise do Espalhamento de Caracteristicas pela Interpretacao Visual de Rastros de Execucao</t>
   </si>
   <si>
@@ -431,9 +410,6 @@
     <t>André Amâncio; Rodrigo Santos; Paulo Parreira Junior; Heitor Costa; Cláudia Werner; Antônio Resende; Fábio Silveira</t>
   </si>
   <si>
-    <t>UFLA; COPPE/UFRJ; UFSCar; UFMG; UNIFESP</t>
-  </si>
-  <si>
     <t>Estimativa de Métricas de Separacão de Interesses em Processos de Refatoracão para Extração de Aspectos</t>
   </si>
   <si>
@@ -494,9 +470,6 @@
     <t>Guilherme Zanetti Kümmel</t>
   </si>
   <si>
-    <t>NOVAPROLINK – Empresa de Desenvolvimento de Softwares</t>
-  </si>
-  <si>
     <t>Modelo de Gestão de Demandas de Manutenção de Software: a Experiência da PUC Minas</t>
   </si>
   <si>
@@ -539,18 +512,12 @@
     <t>Cláudia Werner; Leonardo Murta; Chessman Corrêa; Rodrigo Santos; João Gustavo Prudêncio; Paula Fernandes; Marcelo Schots; Rafael Cepêda; Flávio Lyra</t>
   </si>
   <si>
-    <t>COPPE/UFRJ; UFF; CEPEL</t>
-  </si>
-  <si>
     <t>Verificacao de aderencia entre arquiteturas conceituais e emergentes utilizando a abordagem PREViA</t>
   </si>
   <si>
     <t>Marcelo Schots; Marlon Silva; Leonardo Murta; Cláudia Werner</t>
   </si>
   <si>
-    <t>COPPE/UFRJ; UFF</t>
-  </si>
-  <si>
     <t>Observando Evolucao de Software atraves de Modelos Dinamicos</t>
   </si>
   <si>
@@ -698,9 +665,6 @@
     <t>Eliana Kaneshima; Maria Cristina Neves de Oliveira; Rosana Teresinha Vaccare Braga</t>
   </si>
   <si>
-    <t>Embrapa Soja; USP</t>
-  </si>
-  <si>
     <t>Uma Proposta de Múltiplas Visões Coordenadas para Apoiar Análise de Impacto de Mudança</t>
   </si>
   <si>
@@ -725,9 +689,6 @@
     <t>Maria Istela Cagnin; Marcelo A. Santos Turine; Márcio A. I. Silva; Geraldo B. Landre; Leandro M. Oliveira; Vitor M. A. Lima; Maxwell S. Santos; Débora M. B. Paiva; Camilo Carromeu</t>
   </si>
   <si>
-    <t>UFMS; Embrapa Gado de Corte</t>
-  </si>
-  <si>
     <t>Metamodelo para Integração de Ferramentas de Mineração de Interesses Transversais e de Visualização de Software</t>
   </si>
   <si>
@@ -770,18 +731,12 @@
     <t>Thiago Amorim Pereira; Marcelo Schots</t>
   </si>
   <si>
-    <t>UERJ; COPPE/UFRJ</t>
-  </si>
-  <si>
     <t>EvolTrack: A Plug-in-Based Infrastructure for Visualizing Software Evolution</t>
   </si>
   <si>
     <t>Cláudia Werner; Leonardo Murta; Marcelo Schots; Andréa M. Magdaleno; Marlon Silva; Rafael Cepêda; Caio Vahia</t>
   </si>
   <si>
-    <t>COPPE/UFRJ; UFF; UNIRIO</t>
-  </si>
-  <si>
     <t>Visualização da evolução de software com XFlow: Integrando aspectos técnicos e sociais em múltiplas visualizações</t>
   </si>
   <si>
@@ -893,9 +848,6 @@
     <t>Michel Araújo Vasconcelos; Davi Monteiro Barbosa; Paulo Henrique M. Maia; Nabor C. Mendonça</t>
   </si>
   <si>
-    <t>UECE; UNIFOR; Centro Universitário Estácio do Ceará</t>
-  </si>
-  <si>
     <t>What Questions Developers Ask During Software Evolution? An Academic Perspective</t>
   </si>
   <si>
@@ -1163,9 +1115,6 @@
     <t>UFMG; CEFET-MG</t>
   </si>
   <si>
-    <t>COPPE/UFRJ; UERJ; UFJF</t>
-  </si>
-  <si>
     <t>UFBA; IFBA; UNIFACS</t>
   </si>
   <si>
@@ -1497,6 +1446,282 @@
   </si>
   <si>
     <t>UFLA; UFSJ</t>
+  </si>
+  <si>
+    <t>How do Technical Factors Affect Developers in Mobile Software Ecosystems</t>
+  </si>
+  <si>
+    <t>Caio Steglich; Sabrina Marczak; Rodrigo Santos; Luiz Guerra; Luiz Mosmann; Cleidson de Souza; Fernando Figueira Filho; Marcelo Perin</t>
+  </si>
+  <si>
+    <t>Uma Investigação da Aplicação de Aprendizado de Máquina para Detecção de Smells Arquiteturais</t>
+  </si>
+  <si>
+    <t>Warteruzannan Soyer Cunha; Valter Vieira de Camargo</t>
+  </si>
+  <si>
+    <t>O Impacto da Utilização da Ferramenta Pivotal Tracker para Monitoração de Desempenho em Times Ágeis de Desenvolvimento de Software</t>
+  </si>
+  <si>
+    <t>Dorgival Netto; Ana de Holanda; Flavio Neves; Cloves Rocha; Helena Bastos</t>
+  </si>
+  <si>
+    <t>Um estudo preliminar sobre o uso de uma arquitetura deep learning para seleção de respostas no problema de recuperação de código-fonte</t>
+  </si>
+  <si>
+    <t>Marcelo de Rezende Martins; Marco Aurélio Gerosa</t>
+  </si>
+  <si>
+    <t>Análise de Sentimentos em Discussões de Issues Reabertas do Github</t>
+  </si>
+  <si>
+    <t>Gláucya Boechat; Joselito Mota Jr; Ivan Machado; Manoel Mendonça</t>
+  </si>
+  <si>
+    <t>BULNER: BUg Localization with word embeddings and NEtwork Regularization</t>
+  </si>
+  <si>
+    <t>Jacson Rodrigues Barbosa; Ricardo Marcondes Marcacini; Ricardo Britto; Frederico Soares; Solange Rezende; Auri M. R. Vincenzi; Márcio E. Delamaro</t>
+  </si>
+  <si>
+    <t>Análise e melhoria do processo de reengenharia de software: um estudo de caso</t>
+  </si>
+  <si>
+    <t>Guilherme Mendonça de Moraes; Edgard Costa Oliveira</t>
+  </si>
+  <si>
+    <t>Uma análise da relação entre code smells e dívida técnica auto-admitida</t>
+  </si>
+  <si>
+    <t>Felipe Gustavo de S. Gomes; Thiago Souto Mendes; Rodrigo O. Spínola; Manoel Mendonça; Mário Farias</t>
+  </si>
+  <si>
+    <t>Clustering Similarity Measures for Architecture Recovery of Evolving Software</t>
+  </si>
+  <si>
+    <t>Douglas E. U. Silva; Roberto A. Bittencourt; Rodrigo T. Calumby</t>
+  </si>
+  <si>
+    <t>How Workspaces Influence Software Development? Preliminary Results of a Systematic Literature Review</t>
+  </si>
+  <si>
+    <t>Victor G. J. Costa; Cesár França</t>
+  </si>
+  <si>
+    <t>Um relato sobre a migração de uma plataforma de offloading para microsserviços</t>
+  </si>
+  <si>
+    <t>Adriano L. Cândido; Fernando A. M. Trinta; Paulo A. L. Rego; Lincoln S Rocha; Nabor C. Mendonça; Vinicius C. Garcia</t>
+  </si>
+  <si>
+    <t>Visualizing the Maintainability of Feature Models in SPLs</t>
+  </si>
+  <si>
+    <t>Luan Lima; Anderson Uchôa; Carla Bezerra; Emanuel Coutinho; Lincoln Rocha</t>
+  </si>
+  <si>
+    <t>Analisando Estratégias para Identificação de Dívidas Técnicas</t>
+  </si>
+  <si>
+    <t>Isabela Oliveira; Humberto T. Marques-Neto; Laerte Xavier</t>
+  </si>
+  <si>
+    <t>Proposta de uma abordagem para decompor sistemas monolíticos em microsserviços</t>
+  </si>
+  <si>
+    <t>Felipe Chateaubriand Brasil; Ricardo Terra</t>
+  </si>
+  <si>
+    <t>Data-Flow Analysis Heuristic for Vulnerability Detection on Configurable Systems</t>
+  </si>
+  <si>
+    <t>Gleyberson Andrade; Elder Cirilo; Vinicius Durelli; Bruno Cafeo; Eiji Adachi</t>
+  </si>
+  <si>
+    <t>Quero lhe usar! Uma Análise do Público Alvo de Code Samples</t>
+  </si>
+  <si>
+    <t>Willian Braga; Gabriel Menezes; Awdren Fontão; André Hora; Bruno Cafeo</t>
+  </si>
+  <si>
+    <t>Validação e construção de um dicionário léxico para auxiliar a análise de sentimentos em repositórios de projetos de software</t>
+  </si>
+  <si>
+    <t>Hiolanda Menezes; Gláucya Boechat; Joselito Mota Jr; Ivan Machado</t>
+  </si>
+  <si>
+    <t>Contextual Similarity Among Identifier Names: An Empirical Study</t>
+  </si>
+  <si>
+    <t>Remo Gresta; Elder Cirilo</t>
+  </si>
+  <si>
+    <t>DiffMutAnalyze: uma ferramenta para auxiliar a análise dos mutantes equivalentes no ensino do teste de mutação</t>
+  </si>
+  <si>
+    <t>Juliana Botelho; Maurício Souza; Vinicius H. S. Durelli; Rafael S. Durelli</t>
+  </si>
+  <si>
+    <t>Caracterizando a evolução de software de contratos inteligentes: Um estudo exploratório-descritivo utilizando GitHub e Etherscan</t>
+  </si>
+  <si>
+    <t>Alan Rodrigues; Allysson Allex Araújo; Matheus Paixao; Pamella Soares</t>
+  </si>
+  <si>
+    <t>What do software team managers want from a skills identification?</t>
+  </si>
+  <si>
+    <t>Matheus A. Flauzino; Mauricio R. D. A. Souza; Vinicius H. S. Durelli; Rafael S. Durelli</t>
+  </si>
+  <si>
+    <t>Minerando Motivações para Aplicação de Extract Method: Um Estudo Preliminar</t>
+  </si>
+  <si>
+    <t>Jalisson Henrique; Marcos Dósea; Cláudio Sant’Anna</t>
+  </si>
+  <si>
+    <t>Investigating vulnerability datasets</t>
+  </si>
+  <si>
+    <t>Rodrigo Andrade; Vinícius Santos</t>
+  </si>
+  <si>
+    <t>Revealing Developers’ Arguments on Validating the Incidence of Code Smells: A Focus Group Experience</t>
+  </si>
+  <si>
+    <t>Luis Felipi Junionello; Rafael de Mello; Roberto Oliveira; Leonardo Sousa; Alexander López; Alessandro Garcia</t>
+  </si>
+  <si>
+    <t>Uma Análise da Co-Evolução de Teste em Projetos de Software no GitHub</t>
+  </si>
+  <si>
+    <t>Charles Miranda; Guilherme Avelino; Pedro Santos Neto; Victor da Silva</t>
+  </si>
+  <si>
+    <t>BOHR - Uma Ferramenta para a Identificação de Átomos de Confusão em Códigos Java</t>
+  </si>
+  <si>
+    <t>Wendell Mendes; Windson Viana; Lincoln Rocha</t>
+  </si>
+  <si>
+    <t>Readability and Understandability Scores for Snippet Assessment: an Exploratory Study</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo C. Dantas; Marcelo A. Maia</t>
+  </si>
+  <si>
+    <t>Say my name! An empirical study on the pronounceability of identifier names</t>
+  </si>
+  <si>
+    <t>Bad Smells in Javascript - A Mapping Study</t>
+  </si>
+  <si>
+    <t>Aryclenio Xavier Barros; Eiji Adachi</t>
+  </si>
+  <si>
+    <t>Assessing the Occurrence of Blocking Operations in Database Schema Evolution: A Case Study</t>
+  </si>
+  <si>
+    <t>Willie Lawrence; Eiji Adachi</t>
+  </si>
+  <si>
+    <t>USP; UFSCar; UFMS; Ericsson; UFG; TJGO</t>
+  </si>
+  <si>
+    <t>UFC; UNIFOR; UFPE; FVS</t>
+  </si>
+  <si>
+    <t>UFBA; IFBA; UNIFACS; IFS</t>
+  </si>
+  <si>
+    <t>UEFS</t>
+  </si>
+  <si>
+    <t>CESAR; UFRPE</t>
+  </si>
+  <si>
+    <t>UNB</t>
+  </si>
+  <si>
+    <t>PUCRS; UNIRIO; UFPA; UFRN</t>
+  </si>
+  <si>
+    <t>UFPE; IFMS; IFAC</t>
+  </si>
+  <si>
+    <t>UFC; PUC Rio</t>
+  </si>
+  <si>
+    <t>UFSJ; UFMS; UFRN</t>
+  </si>
+  <si>
+    <t>UFMS; UFMG</t>
+  </si>
+  <si>
+    <t>UFSJ</t>
+  </si>
+  <si>
+    <t>UFC; UECE</t>
+  </si>
+  <si>
+    <t>UFAPE</t>
+  </si>
+  <si>
+    <t>CEFET-RJ; UEG; CMU; CERTI; PUC Rio</t>
+  </si>
+  <si>
+    <t>UFPI</t>
+  </si>
+  <si>
+    <t>UFRJ</t>
+  </si>
+  <si>
+    <t>UFRJ; CEFET Campos</t>
+  </si>
+  <si>
+    <t>UFLA; UFRJ</t>
+  </si>
+  <si>
+    <t>UFLA; UFRJ; UFSCar; UFMG; UNIFESP</t>
+  </si>
+  <si>
+    <t>UFRJ; UFF; CEPEL</t>
+  </si>
+  <si>
+    <t>UFRJ; UFF</t>
+  </si>
+  <si>
+    <t>UERJ; UFRJ</t>
+  </si>
+  <si>
+    <t>UFRJ; UFF; UNIRIO</t>
+  </si>
+  <si>
+    <t>UFRJ; UERJ; UFJF</t>
+  </si>
+  <si>
+    <t>UNIGOIÁS</t>
+  </si>
+  <si>
+    <t>BB; UCB</t>
+  </si>
+  <si>
+    <t>SERPRO; CPQD</t>
+  </si>
+  <si>
+    <t>UFMG; UFU; Google</t>
+  </si>
+  <si>
+    <t>NOVAPROLINK</t>
+  </si>
+  <si>
+    <t>Embrapa; USP</t>
+  </si>
+  <si>
+    <t>UFMS; Embrapa</t>
+  </si>
+  <si>
+    <t>UECE; UNIFOR; Estácio</t>
   </si>
 </sst>
 </file>
@@ -3658,10 +3883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:E221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="G182" sqref="G182"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3696,10 +3921,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>2004</v>
@@ -3707,16 +3932,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>2004</v>
@@ -3724,16 +3949,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>2004</v>
@@ -3741,16 +3966,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>2004</v>
@@ -3758,16 +3983,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>555</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>2004</v>
@@ -3775,16 +4000,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>2004</v>
@@ -3792,16 +4017,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>547</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <v>2004</v>
@@ -3809,16 +4034,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>2005</v>
@@ -3826,16 +4051,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>2005</v>
@@ -3843,16 +4068,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>547</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <v>2005</v>
@@ -3860,16 +4085,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <v>2005</v>
@@ -3877,16 +4102,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>556</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <v>2005</v>
@@ -3894,16 +4119,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <v>2005</v>
@@ -3911,16 +4136,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>2005</v>
@@ -3928,16 +4153,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16">
         <v>2005</v>
@@ -3945,16 +4170,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17">
         <v>2005</v>
@@ -3962,16 +4187,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18">
         <v>2005</v>
@@ -3979,16 +4204,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19">
         <v>2005</v>
@@ -3996,16 +4221,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>2005</v>
@@ -4013,16 +4238,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21">
         <v>2006</v>
@@ -4030,16 +4255,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>2006</v>
@@ -4047,16 +4272,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>2006</v>
@@ -4064,16 +4289,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <v>2006</v>
@@ -4081,16 +4306,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25">
         <v>2006</v>
@@ -4098,16 +4323,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>2006</v>
@@ -4115,16 +4340,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>557</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27">
         <v>2006</v>
@@ -4132,16 +4357,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28">
         <v>2006</v>
@@ -4149,16 +4374,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29">
         <v>2006</v>
@@ -4166,16 +4391,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30">
         <v>2007</v>
@@ -4183,16 +4408,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31">
         <v>2007</v>
@@ -4200,16 +4425,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32">
         <v>2007</v>
@@ -4217,16 +4442,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>558</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33">
         <v>2007</v>
@@ -4234,16 +4459,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34">
         <v>2007</v>
@@ -4251,16 +4476,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35">
         <v>2007</v>
@@ -4268,16 +4493,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E36">
         <v>2007</v>
@@ -4285,16 +4510,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37">
         <v>2007</v>
@@ -4302,16 +4527,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E38">
         <v>2007</v>
@@ -4319,16 +4544,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E39">
         <v>2008</v>
@@ -4336,16 +4561,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>548</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40">
         <v>2008</v>
@@ -4353,16 +4578,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41">
         <v>2008</v>
@@ -4370,16 +4595,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <v>2008</v>
@@ -4387,16 +4612,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43">
         <v>2008</v>
@@ -4404,16 +4629,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44">
         <v>2008</v>
@@ -4421,16 +4646,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E45">
         <v>2008</v>
@@ -4438,16 +4663,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>547</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E46">
         <v>2008</v>
@@ -4455,16 +4680,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E47">
         <v>2009</v>
@@ -4472,16 +4697,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E48">
         <v>2009</v>
@@ -4489,16 +4714,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E49">
         <v>2009</v>
@@ -4506,16 +4731,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>549</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50">
         <v>2009</v>
@@ -4523,16 +4748,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E51">
         <v>2009</v>
@@ -4540,16 +4765,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52">
         <v>2009</v>
@@ -4557,16 +4782,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53">
         <v>2009</v>
@@ -4574,16 +4799,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E54">
         <v>2009</v>
@@ -4591,16 +4816,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E55">
         <v>2009</v>
@@ -4608,16 +4833,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B56" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E56">
         <v>2009</v>
@@ -4625,16 +4850,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E57">
         <v>2009</v>
@@ -4642,16 +4867,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>559</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58">
         <v>2009</v>
@@ -4659,16 +4884,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C59" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E59">
         <v>2009</v>
@@ -4676,16 +4901,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C60" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E60">
         <v>2010</v>
@@ -4693,16 +4918,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C61" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E61">
         <v>2010</v>
@@ -4710,16 +4935,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E62">
         <v>2010</v>
@@ -4727,16 +4952,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C63" t="s">
-        <v>168</v>
+        <v>550</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E63">
         <v>2010</v>
@@ -4744,16 +4969,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B64" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C64" t="s">
-        <v>171</v>
+        <v>551</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64">
         <v>2010</v>
@@ -4761,16 +4986,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E65">
         <v>2010</v>
@@ -4778,16 +5003,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B66" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C66" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E66">
         <v>2010</v>
@@ -4795,16 +5020,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B67" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E67">
         <v>2010</v>
@@ -4812,16 +5037,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B68" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C68" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E68">
         <v>2010</v>
@@ -4829,16 +5054,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B69" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C69" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E69">
         <v>2010</v>
@@ -4846,16 +5071,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B70" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C70" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E70">
         <v>2010</v>
@@ -4863,16 +5088,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B71" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D71" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E71">
         <v>2011</v>
@@ -4880,16 +5105,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E72">
         <v>2011</v>
@@ -4897,16 +5122,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C73" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D73" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E73">
         <v>2011</v>
@@ -4914,16 +5139,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B74" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C74" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E74">
         <v>2011</v>
@@ -4931,16 +5156,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B75" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C75" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E75">
         <v>2011</v>
@@ -4948,16 +5173,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B76" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C76" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="D76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76">
         <v>2011</v>
@@ -4965,16 +5190,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B77" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C77" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D77" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E77">
         <v>2012</v>
@@ -4982,16 +5207,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B78" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E78">
         <v>2012</v>
@@ -4999,16 +5224,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B79" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E79">
         <v>2012</v>
@@ -5016,16 +5241,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B80" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="C80" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D80" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E80">
         <v>2012</v>
@@ -5033,16 +5258,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B81" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D81" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E81">
         <v>2012</v>
@@ -5050,16 +5275,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B82" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C82" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D82" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E82">
         <v>2012</v>
@@ -5067,16 +5292,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B83" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D83" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E83">
         <v>2012</v>
@@ -5084,16 +5309,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B84" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C84" t="s">
-        <v>221</v>
+        <v>560</v>
       </c>
       <c r="D84" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E84">
         <v>2013</v>
@@ -5101,16 +5326,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B85" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C85" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D85" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E85">
         <v>2013</v>
@@ -5118,16 +5343,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B86" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C86" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E86">
         <v>2013</v>
@@ -5135,16 +5360,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="B87" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C87" t="s">
-        <v>230</v>
+        <v>561</v>
       </c>
       <c r="D87" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E87">
         <v>2013</v>
@@ -5152,16 +5377,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="C88" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E88">
         <v>2013</v>
@@ -5169,16 +5394,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="B89" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C89" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E89">
         <v>2013</v>
@@ -5186,16 +5411,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B90" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="C90" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D90" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E90">
         <v>2011</v>
@@ -5203,16 +5428,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C91" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="D91" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E91">
         <v>2011</v>
@@ -5220,16 +5445,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B92" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C92" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D92" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E92">
         <v>2011</v>
@@ -5237,16 +5462,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B93" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C93" t="s">
-        <v>245</v>
+        <v>552</v>
       </c>
       <c r="D93" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E93">
         <v>2011</v>
@@ -5254,16 +5479,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B94" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C94" t="s">
-        <v>248</v>
+        <v>553</v>
       </c>
       <c r="D94" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E94">
         <v>2011</v>
@@ -5271,16 +5496,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B95" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C95" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="D95" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E95">
         <v>2011</v>
@@ -5288,16 +5513,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B96" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C96" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D96" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E96">
         <v>2011</v>
@@ -5305,16 +5530,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B97" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C97" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D97" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E97">
         <v>2012</v>
@@ -5322,16 +5547,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B98" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="C98" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="D98" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E98">
         <v>2012</v>
@@ -5339,16 +5564,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B99" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C99" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="D99" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E99">
         <v>2012</v>
@@ -5356,16 +5581,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="B100" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="C100" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="D100" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E100">
         <v>2012</v>
@@ -5373,16 +5598,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B101" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C101" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="D101" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E101">
         <v>2012</v>
@@ -5390,16 +5615,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="B102" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C102" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D102" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E102">
         <v>2012</v>
@@ -5407,16 +5632,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="B103" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="C103" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D103" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E103">
         <v>2013</v>
@@ -5424,16 +5649,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="B104" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="C104" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D104" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E104">
         <v>2013</v>
@@ -5441,16 +5666,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B105" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C105" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D105" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E105">
         <v>2013</v>
@@ -5458,16 +5683,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B106" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C106" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="D106" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E106">
         <v>2013</v>
@@ -5475,16 +5700,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="B107" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C107" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D107" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E107">
         <v>2013</v>
@@ -5492,16 +5717,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="B108" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C108" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D108" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E108">
         <v>2013</v>
@@ -5509,16 +5734,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="B109" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="C109" t="s">
-        <v>286</v>
+        <v>562</v>
       </c>
       <c r="D109" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E109">
         <v>2013</v>
@@ -5526,16 +5751,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B110" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="C110" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="D110" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E110">
         <v>2014</v>
@@ -5543,16 +5768,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="B111" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="C111" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D111" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E111">
         <v>2014</v>
@@ -5560,16 +5785,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="B112" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="C112" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D112" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E112">
         <v>2014</v>
@@ -5577,16 +5802,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B113" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="C113" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="D113" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E113">
         <v>2014</v>
@@ -5594,16 +5819,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="B114" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="C114" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="D114" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E114">
         <v>2014</v>
@@ -5611,16 +5836,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="B115" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="C115" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D115" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E115">
         <v>2014</v>
@@ -5628,16 +5853,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="B116" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="C116" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D116" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E116">
         <v>2014</v>
@@ -5645,16 +5870,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="B117" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="C117" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D117" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E117">
         <v>2014</v>
@@ -5662,16 +5887,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B118" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="C118" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D118" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E118">
         <v>2014</v>
@@ -5679,16 +5904,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="B119" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="C119" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="D119" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E119">
         <v>2014</v>
@@ -5696,16 +5921,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B120" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="C120" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D120" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E120">
         <v>2014</v>
@@ -5713,16 +5938,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="B121" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C121" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="D121" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E121">
         <v>2014</v>
@@ -5730,16 +5955,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="B122" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="C122" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D122" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E122">
         <v>2014</v>
@@ -5747,16 +5972,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="B123" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="C123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D123" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E123">
         <v>2014</v>
@@ -5764,16 +5989,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="B124" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="C124" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D124" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E124">
         <v>2015</v>
@@ -5781,16 +6006,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="B125" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="C125" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D125" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E125">
         <v>2015</v>
@@ -5798,16 +6023,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="B126" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="C126" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="D126" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E126">
         <v>2015</v>
@@ -5815,16 +6040,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="B127" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="C127" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D127" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E127">
         <v>2015</v>
@@ -5832,16 +6057,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="B128" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="C128" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D128" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E128">
         <v>2015</v>
@@ -5849,16 +6074,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="B129" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="C129" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D129" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E129">
         <v>2015</v>
@@ -5866,16 +6091,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="B130" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="C130" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D130" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E130">
         <v>2015</v>
@@ -5883,16 +6108,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="B131" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="C131" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D131" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E131">
         <v>2015</v>
@@ -5900,16 +6125,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="B132" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="C132" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D132" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E132">
         <v>2015</v>
@@ -5917,16 +6142,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="B133" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="C133" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D133" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E133">
         <v>2015</v>
@@ -5934,16 +6159,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="B134" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C134" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="D134" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E134">
         <v>2015</v>
@@ -5951,16 +6176,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="B135" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="C135" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="D135" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E135">
         <v>2015</v>
@@ -5968,16 +6193,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="C136" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D136" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E136">
         <v>2015</v>
@@ -5985,16 +6210,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="B137" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="C137" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D137" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E137">
         <v>2015</v>
@@ -6002,16 +6227,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="B138" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="C138" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="D138" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E138">
         <v>2015</v>
@@ -6019,16 +6244,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="B139" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="C139" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="D139" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E139">
         <v>2016</v>
@@ -6036,16 +6261,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B140" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="C140" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="D140" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E140">
         <v>2016</v>
@@ -6053,16 +6278,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="B141" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="C141" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="D141" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E141">
         <v>2016</v>
@@ -6070,16 +6295,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B142" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="C142" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="D142" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E142">
         <v>2016</v>
@@ -6087,16 +6312,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="B143" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
       <c r="C143" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D143" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E143">
         <v>2016</v>
@@ -6104,16 +6329,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="B144" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="C144" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D144" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E144">
         <v>2016</v>
@@ -6121,16 +6346,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="B145" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
       <c r="C145" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="D145" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E145">
         <v>2016</v>
@@ -6138,16 +6363,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="B146" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="C146" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D146" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E146">
         <v>2016</v>
@@ -6155,16 +6380,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="B147" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
       <c r="C147" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D147" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E147">
         <v>2016</v>
@@ -6172,16 +6397,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="B148" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="C148" t="s">
-        <v>376</v>
+        <v>554</v>
       </c>
       <c r="D148" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E148">
         <v>2016</v>
@@ -6189,16 +6414,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="B149" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
       <c r="C149" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="D149" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E149">
         <v>2016</v>
@@ -6206,16 +6431,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="B150" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="C150" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="D150" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E150">
         <v>2016</v>
@@ -6223,16 +6448,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="B151" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="C151" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="D151" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E151">
         <v>2016</v>
@@ -6240,16 +6465,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="B152" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="C152" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D152" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E152">
         <v>2016</v>
@@ -6257,16 +6482,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="B153" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="C153" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D153" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E153">
         <v>2016</v>
@@ -6274,16 +6499,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="B154" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="C154" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="D154" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E154">
         <v>2017</v>
@@ -6291,16 +6516,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="B155" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="C155" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D155" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E155">
         <v>2017</v>
@@ -6308,16 +6533,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="B156" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="C156" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="D156" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E156">
         <v>2017</v>
@@ -6325,16 +6550,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="B157" t="s">
-        <v>413</v>
+        <v>396</v>
       </c>
       <c r="C157" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="D157" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E157">
         <v>2017</v>
@@ -6342,16 +6567,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="B158" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="C158" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D158" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E158">
         <v>2017</v>
@@ -6359,16 +6584,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="B159" t="s">
+        <v>391</v>
+      </c>
+      <c r="C159" t="s">
         <v>408</v>
       </c>
-      <c r="C159" t="s">
-        <v>425</v>
-      </c>
       <c r="D159" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E159">
         <v>2017</v>
@@ -6376,16 +6601,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
       <c r="B160" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C160" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="D160" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E160">
         <v>2017</v>
@@ -6393,16 +6618,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="B161" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
       <c r="C161" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="D161" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E161">
         <v>2017</v>
@@ -6410,16 +6635,16 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="B162" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="C162" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="D162" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E162">
         <v>2017</v>
@@ -6427,16 +6652,16 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="B163" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="C163" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="D163" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E163">
         <v>2017</v>
@@ -6444,16 +6669,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="B164" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="C164" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D164" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E164">
         <v>2017</v>
@@ -6461,16 +6686,16 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="B165" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
       <c r="C165" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D165" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E165">
         <v>2017</v>
@@ -6478,16 +6703,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B166" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="C166" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D166" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E166">
         <v>2017</v>
@@ -6495,16 +6720,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="B167" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="C167" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="D167" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E167">
         <v>2017</v>
@@ -6512,16 +6737,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="B168" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
       <c r="C168" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
       <c r="D168" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E168">
         <v>2018</v>
@@ -6529,16 +6754,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="B169" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
       <c r="C169" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D169" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E169">
         <v>2018</v>
@@ -6546,16 +6771,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="B170" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="C170" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D170" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E170">
         <v>2018</v>
@@ -6563,16 +6788,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B171" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
       <c r="C171" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D171" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E171">
         <v>2018</v>
@@ -6580,16 +6805,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B172" t="s">
-        <v>458</v>
+        <v>441</v>
       </c>
       <c r="C172" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="D172" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E172">
         <v>2018</v>
@@ -6597,16 +6822,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="B173" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="C173" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D173" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E173">
         <v>2018</v>
@@ -6614,16 +6839,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>435</v>
+        <v>418</v>
       </c>
       <c r="B174" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="C174" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D174" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E174">
         <v>2018</v>
@@ -6631,16 +6856,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="B175" t="s">
+        <v>444</v>
+      </c>
+      <c r="C175" t="s">
         <v>461</v>
       </c>
-      <c r="C175" t="s">
-        <v>478</v>
-      </c>
       <c r="D175" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E175">
         <v>2018</v>
@@ -6648,16 +6873,16 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
       <c r="B176" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="C176" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D176" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E176">
         <v>2018</v>
@@ -6665,16 +6890,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="B177" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="C177" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="D177" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E177">
         <v>2018</v>
@@ -6682,16 +6907,16 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="B178" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="C178" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="D178" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E178">
         <v>2018</v>
@@ -6699,16 +6924,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="B179" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="C179" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="D179" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E179">
         <v>2018</v>
@@ -6716,16 +6941,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
       <c r="B180" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="C180" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
       <c r="D180" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E180">
         <v>2018</v>
@@ -6733,16 +6958,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="B181" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="C181" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="D181" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E181">
         <v>2018</v>
@@ -6750,16 +6975,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
       <c r="B182" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="C182" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D182" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E182">
         <v>2018</v>
@@ -6767,16 +6992,16 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="B183" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="C183" t="s">
-        <v>7</v>
+        <v>546</v>
       </c>
       <c r="D183" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E183">
         <v>2018</v>
@@ -6784,16 +7009,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="B184" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C184" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D184" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E184">
         <v>2018</v>
@@ -6801,16 +7026,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="B185" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
       <c r="C185" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
       <c r="D185" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E185">
         <v>2018</v>
@@ -6818,16 +7043,16 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="B186" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="C186" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D186" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E186">
         <v>2018</v>
@@ -6835,16 +7060,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="B187" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
       <c r="C187" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D187" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E187">
         <v>2018</v>
@@ -6852,16 +7077,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
       <c r="B188" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
       <c r="C188" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c r="D188" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E188">
         <v>2018</v>
@@ -6869,16 +7094,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="B189" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="C189" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="D189" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E189">
         <v>2018</v>
@@ -6886,16 +7111,16 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="B190" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="C190" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
       <c r="D190" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E190">
         <v>2018</v>
@@ -6903,19 +7128,529 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
       <c r="B191" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C191" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="D191" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E191">
         <v>2018</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>471</v>
+      </c>
+      <c r="B192" t="s">
+        <v>472</v>
+      </c>
+      <c r="C192" t="s">
+        <v>536</v>
+      </c>
+      <c r="D192" t="s">
+        <v>256</v>
+      </c>
+      <c r="E192">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>473</v>
+      </c>
+      <c r="B193" t="s">
+        <v>474</v>
+      </c>
+      <c r="C193" t="s">
+        <v>26</v>
+      </c>
+      <c r="D193" t="s">
+        <v>256</v>
+      </c>
+      <c r="E193">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>475</v>
+      </c>
+      <c r="B194" t="s">
+        <v>476</v>
+      </c>
+      <c r="C194" t="s">
+        <v>537</v>
+      </c>
+      <c r="D194" t="s">
+        <v>256</v>
+      </c>
+      <c r="E194">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>477</v>
+      </c>
+      <c r="B195" t="s">
+        <v>478</v>
+      </c>
+      <c r="C195" t="s">
+        <v>408</v>
+      </c>
+      <c r="D195" t="s">
+        <v>256</v>
+      </c>
+      <c r="E195">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>479</v>
+      </c>
+      <c r="B196" t="s">
+        <v>480</v>
+      </c>
+      <c r="C196" t="s">
+        <v>168</v>
+      </c>
+      <c r="D196" t="s">
+        <v>256</v>
+      </c>
+      <c r="E196">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>481</v>
+      </c>
+      <c r="B197" t="s">
+        <v>482</v>
+      </c>
+      <c r="C197" t="s">
+        <v>530</v>
+      </c>
+      <c r="D197" t="s">
+        <v>256</v>
+      </c>
+      <c r="E197">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>483</v>
+      </c>
+      <c r="B198" t="s">
+        <v>484</v>
+      </c>
+      <c r="C198" t="s">
+        <v>535</v>
+      </c>
+      <c r="D198" t="s">
+        <v>256</v>
+      </c>
+      <c r="E198">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>485</v>
+      </c>
+      <c r="B199" t="s">
+        <v>486</v>
+      </c>
+      <c r="C199" t="s">
+        <v>532</v>
+      </c>
+      <c r="D199" t="s">
+        <v>256</v>
+      </c>
+      <c r="E199">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>487</v>
+      </c>
+      <c r="B200" t="s">
+        <v>488</v>
+      </c>
+      <c r="C200" t="s">
+        <v>533</v>
+      </c>
+      <c r="D200" t="s">
+        <v>256</v>
+      </c>
+      <c r="E200">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>489</v>
+      </c>
+      <c r="B201" t="s">
+        <v>490</v>
+      </c>
+      <c r="C201" t="s">
+        <v>534</v>
+      </c>
+      <c r="D201" t="s">
+        <v>256</v>
+      </c>
+      <c r="E201">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>491</v>
+      </c>
+      <c r="B202" t="s">
+        <v>492</v>
+      </c>
+      <c r="C202" t="s">
+        <v>531</v>
+      </c>
+      <c r="D202" t="s">
+        <v>256</v>
+      </c>
+      <c r="E202">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>493</v>
+      </c>
+      <c r="B203" t="s">
+        <v>494</v>
+      </c>
+      <c r="C203" t="s">
+        <v>538</v>
+      </c>
+      <c r="D203" t="s">
+        <v>256</v>
+      </c>
+      <c r="E203">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>495</v>
+      </c>
+      <c r="B204" t="s">
+        <v>496</v>
+      </c>
+      <c r="C204" t="s">
+        <v>147</v>
+      </c>
+      <c r="D204" t="s">
+        <v>256</v>
+      </c>
+      <c r="E204">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>497</v>
+      </c>
+      <c r="B205" t="s">
+        <v>498</v>
+      </c>
+      <c r="C205" t="s">
+        <v>410</v>
+      </c>
+      <c r="D205" t="s">
+        <v>256</v>
+      </c>
+      <c r="E205">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>499</v>
+      </c>
+      <c r="B206" t="s">
+        <v>500</v>
+      </c>
+      <c r="C206" t="s">
+        <v>539</v>
+      </c>
+      <c r="D206" t="s">
+        <v>256</v>
+      </c>
+      <c r="E206">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>501</v>
+      </c>
+      <c r="B207" t="s">
+        <v>502</v>
+      </c>
+      <c r="C207" t="s">
+        <v>540</v>
+      </c>
+      <c r="D207" t="s">
+        <v>256</v>
+      </c>
+      <c r="E207">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>503</v>
+      </c>
+      <c r="B208" t="s">
+        <v>504</v>
+      </c>
+      <c r="C208" t="s">
+        <v>168</v>
+      </c>
+      <c r="D208" t="s">
+        <v>256</v>
+      </c>
+      <c r="E208">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>505</v>
+      </c>
+      <c r="B209" t="s">
+        <v>506</v>
+      </c>
+      <c r="C209" t="s">
+        <v>541</v>
+      </c>
+      <c r="D209" t="s">
+        <v>256</v>
+      </c>
+      <c r="E209">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>507</v>
+      </c>
+      <c r="B210" t="s">
+        <v>508</v>
+      </c>
+      <c r="C210" t="s">
+        <v>470</v>
+      </c>
+      <c r="D210" t="s">
+        <v>256</v>
+      </c>
+      <c r="E210">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>509</v>
+      </c>
+      <c r="B211" t="s">
+        <v>510</v>
+      </c>
+      <c r="C211" t="s">
+        <v>542</v>
+      </c>
+      <c r="D211" t="s">
+        <v>256</v>
+      </c>
+      <c r="E211">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>511</v>
+      </c>
+      <c r="B212" t="s">
+        <v>512</v>
+      </c>
+      <c r="C212" t="s">
+        <v>470</v>
+      </c>
+      <c r="D212" t="s">
+        <v>256</v>
+      </c>
+      <c r="E212">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>513</v>
+      </c>
+      <c r="B213" t="s">
+        <v>514</v>
+      </c>
+      <c r="C213" t="s">
+        <v>463</v>
+      </c>
+      <c r="D213" t="s">
+        <v>256</v>
+      </c>
+      <c r="E213">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>515</v>
+      </c>
+      <c r="B214" t="s">
+        <v>516</v>
+      </c>
+      <c r="C214" t="s">
+        <v>543</v>
+      </c>
+      <c r="D214" t="s">
+        <v>256</v>
+      </c>
+      <c r="E214">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>517</v>
+      </c>
+      <c r="B215" t="s">
+        <v>518</v>
+      </c>
+      <c r="C215" t="s">
+        <v>544</v>
+      </c>
+      <c r="D215" t="s">
+        <v>256</v>
+      </c>
+      <c r="E215">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>519</v>
+      </c>
+      <c r="B216" t="s">
+        <v>520</v>
+      </c>
+      <c r="C216" t="s">
+        <v>545</v>
+      </c>
+      <c r="D216" t="s">
+        <v>256</v>
+      </c>
+      <c r="E216">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>521</v>
+      </c>
+      <c r="B217" t="s">
+        <v>522</v>
+      </c>
+      <c r="C217" t="s">
+        <v>329</v>
+      </c>
+      <c r="D217" t="s">
+        <v>256</v>
+      </c>
+      <c r="E217">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>523</v>
+      </c>
+      <c r="B218" t="s">
+        <v>524</v>
+      </c>
+      <c r="C218" t="s">
+        <v>101</v>
+      </c>
+      <c r="D218" t="s">
+        <v>256</v>
+      </c>
+      <c r="E218">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>525</v>
+      </c>
+      <c r="B219" t="s">
+        <v>506</v>
+      </c>
+      <c r="C219" t="s">
+        <v>541</v>
+      </c>
+      <c r="D219" t="s">
+        <v>256</v>
+      </c>
+      <c r="E219">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>526</v>
+      </c>
+      <c r="B220" t="s">
+        <v>527</v>
+      </c>
+      <c r="C220" t="s">
+        <v>468</v>
+      </c>
+      <c r="D220" t="s">
+        <v>256</v>
+      </c>
+      <c r="E220">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>528</v>
+      </c>
+      <c r="B221" t="s">
+        <v>529</v>
+      </c>
+      <c r="C221" t="s">
+        <v>468</v>
+      </c>
+      <c r="D221" t="s">
+        <v>256</v>
+      </c>
+      <c r="E221">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds VEM 2022 data
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/vem2004-2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/vem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EA200F-4D6C-1B47-B43D-70CD5B89875D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82360055-65AC-7D4C-AE7D-035D571493A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="589">
   <si>
     <t>title</t>
   </si>
@@ -416,9 +416,6 @@
     <t>César Francisco de Moura Couto; Jaqueline Faria de Oliveira; Marco Tulio Valente</t>
   </si>
   <si>
-    <t>CEFET Minas; PUC Minas</t>
-  </si>
-  <si>
     <t>Reestruturação de um Framework de Aplicação com um Framework Transversal de Persistência</t>
   </si>
   <si>
@@ -938,9 +935,6 @@
     <t>Henrique Nunes Gomes, Mariza Bigonha, Kecia Ferreira; Flávio Madureira</t>
   </si>
   <si>
-    <t>UFMG; CEFET Minas</t>
-  </si>
-  <si>
     <t>Uma Análise da História do VEM, WBVS e WMSWM</t>
   </si>
   <si>
@@ -1722,6 +1716,90 @@
   </si>
   <si>
     <t>UECE; UNIFOR; Estácio</t>
+  </si>
+  <si>
+    <t>Avaliação de Ferramentas de Identificação de Dívida Técnica Auto-Admitida</t>
+  </si>
+  <si>
+    <t>Como os mantenedores usam GitHub Reactions? Um estudo exploratório</t>
+  </si>
+  <si>
+    <t>ConCAD: A Tool for Interactive Code Anomaly Detection</t>
+  </si>
+  <si>
+    <t>Democracia em Xeque: Um Estudo Comparativo sobre Detecção de Code Smells</t>
+  </si>
+  <si>
+    <t>Divinator: A Visual Studio Code Extension to Source Code Summarization</t>
+  </si>
+  <si>
+    <t>Empirical investigation of the influence of continuous integration bad practices on software quality</t>
+  </si>
+  <si>
+    <t>Entendendo o engajamento das comunidades front-end e back-end nos repositórios do GitHub</t>
+  </si>
+  <si>
+    <t>Exploring Pull Requests in Code Samples</t>
+  </si>
+  <si>
+    <t>Merge Nature: a tool to support research about merge conflicts</t>
+  </si>
+  <si>
+    <t>Perceptions and Difficulties of Software Engineering Students in Code Smells Refactoring</t>
+  </si>
+  <si>
+    <t>Using Controllers to Adapt Messaging Systems: An Initial Experience</t>
+  </si>
+  <si>
+    <t>Danyllo Albuquerque; Felipe Silva; Mirko Perkusich; Hyggo Almeida; Angelo Perkusich</t>
+  </si>
+  <si>
+    <t>UESPI</t>
+  </si>
+  <si>
+    <t>Tchalisson Gomes; Alcemir Santos; Diogo Alves</t>
+  </si>
+  <si>
+    <t>Pedro Novais; Hudson Borges; Awdren Fontão; Marco Tulio Valente</t>
+  </si>
+  <si>
+    <t>UFCG; Virtus</t>
+  </si>
+  <si>
+    <t>Henrique Nunes Gomes; Lucas Vegi; Victor Pezzi Gazzinelli Cruz; Eduardo Figueiredo</t>
+  </si>
+  <si>
+    <t>UFMG; UFV</t>
+  </si>
+  <si>
+    <t>Rafael Durelli; Vinicius Durelli; Raphael Bettio; Diego Colombo Dias; Alfredo Goldman</t>
+  </si>
+  <si>
+    <t>UFLA; UFSJ; USP</t>
+  </si>
+  <si>
+    <t>Ruben Blenicio Silva; Carla Ilane Moreira Bezerra</t>
+  </si>
+  <si>
+    <t>Altino Alves Júnior; Letícia de Souza Meireles; Lucas Alves Rossi Figueira; Vítor Marcondes Morais Carmo; Humberto T. Marques-Neto; Laerte Xavier</t>
+  </si>
+  <si>
+    <t>Matheus Melo; Gabriel de Menezes; Bruno Cafeo</t>
+  </si>
+  <si>
+    <t>Luan Ciribelli; João Pedro de Carvalho Lima; Heleno de Souza Campos Junior; Gleiph Ghiotto; Leonardo Murta; Andre Van Der Hoek; Márcio Barros</t>
+  </si>
+  <si>
+    <t>UFJF; UFF; UC Irvine; UNIRIO</t>
+  </si>
+  <si>
+    <t>Humberto Damasceno; João Do Nascimento; Carla Ilane Moreira Bezerra</t>
+  </si>
+  <si>
+    <t>Nelson Rosa; David Mota Cavalcanti</t>
+  </si>
+  <si>
+    <t>CEFET-MG; PUC Minas</t>
   </si>
 </sst>
 </file>
@@ -3883,10 +3961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E221"/>
+  <dimension ref="A1:E232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D222" sqref="D222:D232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3921,7 +3999,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -3989,7 +4067,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -4023,7 +4101,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -4074,7 +4152,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -4108,7 +4186,7 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -4125,7 +4203,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -4142,7 +4220,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -4312,7 +4390,7 @@
         <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -4346,7 +4424,7 @@
         <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -4448,7 +4526,7 @@
         <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -4567,7 +4645,7 @@
         <v>98</v>
       </c>
       <c r="C40" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -4669,7 +4747,7 @@
         <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -4737,7 +4815,7 @@
         <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
@@ -4754,7 +4832,7 @@
         <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>588</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -4765,10 +4843,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" t="s">
         <v>128</v>
-      </c>
-      <c r="B52" t="s">
-        <v>129</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -4782,13 +4860,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" t="s">
         <v>130</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>131</v>
-      </c>
-      <c r="C53" t="s">
-        <v>132</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -4799,13 +4877,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" t="s">
         <v>133</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>134</v>
-      </c>
-      <c r="C54" t="s">
-        <v>135</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -4816,13 +4894,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" t="s">
         <v>136</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>137</v>
-      </c>
-      <c r="C55" t="s">
-        <v>138</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -4833,10 +4911,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" t="s">
         <v>139</v>
-      </c>
-      <c r="B56" t="s">
-        <v>140</v>
       </c>
       <c r="C56" t="s">
         <v>16</v>
@@ -4850,10 +4928,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" t="s">
         <v>141</v>
-      </c>
-      <c r="B57" t="s">
-        <v>142</v>
       </c>
       <c r="C57" t="s">
         <v>13</v>
@@ -4867,13 +4945,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" t="s">
         <v>143</v>
       </c>
-      <c r="B58" t="s">
-        <v>144</v>
-      </c>
       <c r="C58" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -4884,13 +4962,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" t="s">
         <v>145</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>146</v>
-      </c>
-      <c r="C59" t="s">
-        <v>147</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -4901,13 +4979,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
         <v>148</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>149</v>
-      </c>
-      <c r="C60" t="s">
-        <v>150</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -4918,13 +4996,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" t="s">
         <v>151</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>152</v>
-      </c>
-      <c r="C61" t="s">
-        <v>153</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
@@ -4935,13 +5013,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" t="s">
         <v>154</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>155</v>
-      </c>
-      <c r="C62" t="s">
-        <v>156</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -4952,13 +5030,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" t="s">
         <v>157</v>
       </c>
-      <c r="B63" t="s">
-        <v>158</v>
-      </c>
       <c r="C63" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -4969,13 +5047,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" t="s">
         <v>159</v>
       </c>
-      <c r="B64" t="s">
-        <v>160</v>
-      </c>
       <c r="C64" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
@@ -4986,13 +5064,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -5003,13 +5081,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" t="s">
         <v>162</v>
       </c>
-      <c r="B66" t="s">
-        <v>163</v>
-      </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -5020,10 +5098,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" t="s">
         <v>164</v>
-      </c>
-      <c r="B67" t="s">
-        <v>165</v>
       </c>
       <c r="C67" t="s">
         <v>26</v>
@@ -5037,13 +5115,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>165</v>
+      </c>
+      <c r="B68" t="s">
         <v>166</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>167</v>
-      </c>
-      <c r="C68" t="s">
-        <v>168</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
@@ -5054,13 +5132,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>168</v>
+      </c>
+      <c r="B69" t="s">
         <v>169</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>170</v>
-      </c>
-      <c r="C69" t="s">
-        <v>171</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -5071,13 +5149,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>171</v>
+      </c>
+      <c r="B70" t="s">
         <v>172</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>173</v>
-      </c>
-      <c r="C70" t="s">
-        <v>174</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -5088,13 +5166,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>174</v>
+      </c>
+      <c r="B71" t="s">
         <v>175</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>176</v>
-      </c>
-      <c r="C71" t="s">
-        <v>177</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
@@ -5105,13 +5183,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" t="s">
         <v>178</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>179</v>
-      </c>
-      <c r="C72" t="s">
-        <v>180</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -5122,13 +5200,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" t="s">
         <v>181</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>182</v>
-      </c>
-      <c r="C73" t="s">
-        <v>183</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -5139,13 +5217,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>183</v>
+      </c>
+      <c r="B74" t="s">
         <v>184</v>
       </c>
-      <c r="B74" t="s">
-        <v>185</v>
-      </c>
       <c r="C74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
@@ -5156,13 +5234,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>185</v>
+      </c>
+      <c r="B75" t="s">
         <v>186</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>187</v>
-      </c>
-      <c r="C75" t="s">
-        <v>188</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
@@ -5173,13 +5251,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>188</v>
+      </c>
+      <c r="B76" t="s">
         <v>189</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>190</v>
-      </c>
-      <c r="C76" t="s">
-        <v>191</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
@@ -5190,13 +5268,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" t="s">
         <v>192</v>
       </c>
-      <c r="B77" t="s">
-        <v>193</v>
-      </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
@@ -5207,10 +5285,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>193</v>
+      </c>
+      <c r="B78" t="s">
         <v>194</v>
-      </c>
-      <c r="B78" t="s">
-        <v>195</v>
       </c>
       <c r="C78" t="s">
         <v>13</v>
@@ -5224,13 +5302,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>195</v>
+      </c>
+      <c r="B79" t="s">
         <v>196</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>197</v>
-      </c>
-      <c r="C79" t="s">
-        <v>198</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -5241,13 +5319,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" t="s">
         <v>199</v>
       </c>
-      <c r="B80" t="s">
-        <v>200</v>
-      </c>
       <c r="C80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -5258,13 +5336,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>200</v>
+      </c>
+      <c r="B81" t="s">
         <v>201</v>
       </c>
-      <c r="B81" t="s">
-        <v>202</v>
-      </c>
       <c r="C81" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -5275,13 +5353,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>202</v>
+      </c>
+      <c r="B82" t="s">
         <v>203</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>204</v>
-      </c>
-      <c r="C82" t="s">
-        <v>205</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -5292,10 +5370,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" t="s">
         <v>206</v>
-      </c>
-      <c r="B83" t="s">
-        <v>207</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
@@ -5309,13 +5387,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>207</v>
+      </c>
+      <c r="B84" t="s">
         <v>208</v>
       </c>
-      <c r="B84" t="s">
-        <v>209</v>
-      </c>
       <c r="C84" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
@@ -5326,13 +5404,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>209</v>
+      </c>
+      <c r="B85" t="s">
         <v>210</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>211</v>
-      </c>
-      <c r="C85" t="s">
-        <v>212</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
@@ -5343,13 +5421,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>212</v>
+      </c>
+      <c r="B86" t="s">
         <v>213</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>214</v>
-      </c>
-      <c r="C86" t="s">
-        <v>215</v>
       </c>
       <c r="D86" t="s">
         <v>7</v>
@@ -5360,13 +5438,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" t="s">
         <v>216</v>
       </c>
-      <c r="B87" t="s">
-        <v>217</v>
-      </c>
       <c r="C87" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
@@ -5377,13 +5455,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" t="s">
         <v>218</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>219</v>
-      </c>
-      <c r="C88" t="s">
-        <v>220</v>
       </c>
       <c r="D88" t="s">
         <v>7</v>
@@ -5394,13 +5472,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>220</v>
+      </c>
+      <c r="B89" t="s">
         <v>221</v>
       </c>
-      <c r="B89" t="s">
-        <v>222</v>
-      </c>
       <c r="C89" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D89" t="s">
         <v>7</v>
@@ -5411,16 +5489,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>222</v>
+      </c>
+      <c r="B90" t="s">
         <v>223</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>179</v>
+      </c>
+      <c r="D90" t="s">
         <v>224</v>
-      </c>
-      <c r="C90" t="s">
-        <v>180</v>
-      </c>
-      <c r="D90" t="s">
-        <v>225</v>
       </c>
       <c r="E90">
         <v>2011</v>
@@ -5428,16 +5506,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>225</v>
+      </c>
+      <c r="B91" t="s">
         <v>226</v>
       </c>
-      <c r="B91" t="s">
-        <v>227</v>
-      </c>
       <c r="C91" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D91" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E91">
         <v>2011</v>
@@ -5445,16 +5523,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>227</v>
+      </c>
+      <c r="B92" t="s">
         <v>228</v>
       </c>
-      <c r="B92" t="s">
-        <v>229</v>
-      </c>
       <c r="C92" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E92">
         <v>2011</v>
@@ -5462,16 +5540,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>229</v>
+      </c>
+      <c r="B93" t="s">
         <v>230</v>
       </c>
-      <c r="B93" t="s">
-        <v>231</v>
-      </c>
       <c r="C93" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D93" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E93">
         <v>2011</v>
@@ -5479,16 +5557,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>231</v>
+      </c>
+      <c r="B94" t="s">
         <v>232</v>
       </c>
-      <c r="B94" t="s">
-        <v>233</v>
-      </c>
       <c r="C94" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D94" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E94">
         <v>2011</v>
@@ -5496,16 +5574,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>233</v>
+      </c>
+      <c r="B95" t="s">
         <v>234</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>235</v>
       </c>
-      <c r="C95" t="s">
-        <v>236</v>
-      </c>
       <c r="D95" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E95">
         <v>2011</v>
@@ -5513,16 +5591,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>236</v>
+      </c>
+      <c r="B96" t="s">
         <v>237</v>
       </c>
-      <c r="B96" t="s">
-        <v>238</v>
-      </c>
       <c r="C96" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D96" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E96">
         <v>2011</v>
@@ -5530,16 +5608,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>238</v>
+      </c>
+      <c r="B97" t="s">
         <v>239</v>
       </c>
-      <c r="B97" t="s">
-        <v>240</v>
-      </c>
       <c r="C97" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D97" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E97">
         <v>2012</v>
@@ -5547,16 +5625,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>240</v>
+      </c>
+      <c r="B98" t="s">
         <v>241</v>
       </c>
-      <c r="B98" t="s">
-        <v>242</v>
-      </c>
       <c r="C98" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D98" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E98">
         <v>2012</v>
@@ -5564,16 +5642,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>242</v>
+      </c>
+      <c r="B99" t="s">
         <v>243</v>
       </c>
-      <c r="B99" t="s">
-        <v>244</v>
-      </c>
       <c r="C99" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D99" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E99">
         <v>2012</v>
@@ -5581,16 +5659,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>244</v>
+      </c>
+      <c r="B100" t="s">
         <v>245</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>246</v>
       </c>
-      <c r="C100" t="s">
-        <v>247</v>
-      </c>
       <c r="D100" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E100">
         <v>2012</v>
@@ -5598,16 +5676,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>247</v>
+      </c>
+      <c r="B101" t="s">
         <v>248</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>249</v>
       </c>
-      <c r="C101" t="s">
-        <v>250</v>
-      </c>
       <c r="D101" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E101">
         <v>2012</v>
@@ -5615,16 +5693,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>250</v>
+      </c>
+      <c r="B102" t="s">
         <v>251</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>252</v>
       </c>
-      <c r="C102" t="s">
-        <v>253</v>
-      </c>
       <c r="D102" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E102">
         <v>2012</v>
@@ -5632,16 +5710,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>253</v>
+      </c>
+      <c r="B103" t="s">
         <v>254</v>
       </c>
-      <c r="B103" t="s">
-        <v>255</v>
-      </c>
       <c r="C103" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D103" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E103">
         <v>2013</v>
@@ -5649,16 +5727,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>256</v>
+      </c>
+      <c r="B104" t="s">
         <v>257</v>
       </c>
-      <c r="B104" t="s">
-        <v>258</v>
-      </c>
       <c r="C104" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D104" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E104">
         <v>2013</v>
@@ -5666,16 +5744,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>258</v>
+      </c>
+      <c r="B105" t="s">
         <v>259</v>
       </c>
-      <c r="B105" t="s">
-        <v>260</v>
-      </c>
       <c r="C105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E105">
         <v>2013</v>
@@ -5683,16 +5761,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>260</v>
+      </c>
+      <c r="B106" t="s">
         <v>261</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>262</v>
       </c>
-      <c r="C106" t="s">
-        <v>263</v>
-      </c>
       <c r="D106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E106">
         <v>2013</v>
@@ -5700,16 +5778,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>263</v>
+      </c>
+      <c r="B107" t="s">
         <v>264</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>265</v>
       </c>
-      <c r="C107" t="s">
-        <v>266</v>
-      </c>
       <c r="D107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E107">
         <v>2013</v>
@@ -5717,16 +5795,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>266</v>
+      </c>
+      <c r="B108" t="s">
         <v>267</v>
       </c>
-      <c r="B108" t="s">
-        <v>268</v>
-      </c>
       <c r="C108" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D108" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E108">
         <v>2013</v>
@@ -5734,16 +5812,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>268</v>
+      </c>
+      <c r="B109" t="s">
         <v>269</v>
       </c>
-      <c r="B109" t="s">
-        <v>270</v>
-      </c>
       <c r="C109" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E109">
         <v>2013</v>
@@ -5751,16 +5829,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>270</v>
+      </c>
+      <c r="B110" t="s">
         <v>271</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>272</v>
       </c>
-      <c r="C110" t="s">
-        <v>273</v>
-      </c>
       <c r="D110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E110">
         <v>2014</v>
@@ -5768,16 +5846,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>273</v>
+      </c>
+      <c r="B111" t="s">
         <v>274</v>
       </c>
-      <c r="B111" t="s">
-        <v>275</v>
-      </c>
       <c r="C111" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E111">
         <v>2014</v>
@@ -5785,16 +5863,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>275</v>
+      </c>
+      <c r="B112" t="s">
         <v>276</v>
       </c>
-      <c r="B112" t="s">
-        <v>277</v>
-      </c>
       <c r="C112" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D112" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E112">
         <v>2014</v>
@@ -5802,16 +5880,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>277</v>
+      </c>
+      <c r="B113" t="s">
         <v>278</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>279</v>
       </c>
-      <c r="C113" t="s">
-        <v>280</v>
-      </c>
       <c r="D113" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E113">
         <v>2014</v>
@@ -5819,16 +5897,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>280</v>
+      </c>
+      <c r="B114" t="s">
         <v>281</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>282</v>
       </c>
-      <c r="C114" t="s">
-        <v>283</v>
-      </c>
       <c r="D114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E114">
         <v>2014</v>
@@ -5836,16 +5914,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>283</v>
+      </c>
+      <c r="B115" t="s">
         <v>284</v>
       </c>
-      <c r="B115" t="s">
-        <v>285</v>
-      </c>
       <c r="C115" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D115" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E115">
         <v>2014</v>
@@ -5853,16 +5931,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>285</v>
+      </c>
+      <c r="B116" t="s">
         <v>286</v>
       </c>
-      <c r="B116" t="s">
-        <v>287</v>
-      </c>
       <c r="C116" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E116">
         <v>2014</v>
@@ -5870,16 +5948,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>287</v>
+      </c>
+      <c r="B117" t="s">
         <v>288</v>
       </c>
-      <c r="B117" t="s">
-        <v>289</v>
-      </c>
       <c r="C117" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E117">
         <v>2014</v>
@@ -5887,16 +5965,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>289</v>
+      </c>
+      <c r="B118" t="s">
         <v>290</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>291</v>
       </c>
-      <c r="C118" t="s">
-        <v>292</v>
-      </c>
       <c r="D118" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E118">
         <v>2014</v>
@@ -5904,16 +5982,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>292</v>
+      </c>
+      <c r="B119" t="s">
         <v>293</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>294</v>
       </c>
-      <c r="C119" t="s">
-        <v>295</v>
-      </c>
       <c r="D119" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E119">
         <v>2014</v>
@@ -5921,16 +5999,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>295</v>
+      </c>
+      <c r="B120" t="s">
         <v>296</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>297</v>
       </c>
-      <c r="C120" t="s">
-        <v>298</v>
-      </c>
       <c r="D120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E120">
         <v>2014</v>
@@ -5938,16 +6016,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>298</v>
+      </c>
+      <c r="B121" t="s">
         <v>299</v>
       </c>
-      <c r="B121" t="s">
-        <v>300</v>
-      </c>
       <c r="C121" t="s">
-        <v>301</v>
+        <v>357</v>
       </c>
       <c r="D121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E121">
         <v>2014</v>
@@ -5955,16 +6033,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B122" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C122" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E122">
         <v>2014</v>
@@ -5972,16 +6050,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B123" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C123" t="s">
         <v>16</v>
       </c>
       <c r="D123" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E123">
         <v>2014</v>
@@ -5989,16 +6067,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B124" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C124" t="s">
         <v>101</v>
       </c>
       <c r="D124" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E124">
         <v>2015</v>
@@ -6006,16 +6084,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B125" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C125" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D125" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E125">
         <v>2015</v>
@@ -6023,16 +6101,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>308</v>
+      </c>
+      <c r="B126" t="s">
+        <v>309</v>
+      </c>
+      <c r="C126" t="s">
         <v>310</v>
       </c>
-      <c r="B126" t="s">
-        <v>311</v>
-      </c>
-      <c r="C126" t="s">
-        <v>312</v>
-      </c>
       <c r="D126" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E126">
         <v>2015</v>
@@ -6040,16 +6118,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B127" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C127" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D127" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E127">
         <v>2015</v>
@@ -6057,16 +6135,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B128" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C128" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D128" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E128">
         <v>2015</v>
@@ -6074,16 +6152,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B129" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C129" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D129" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E129">
         <v>2015</v>
@@ -6091,16 +6169,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B130" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C130" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D130" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E130">
         <v>2015</v>
@@ -6108,16 +6186,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B131" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C131" t="s">
         <v>13</v>
       </c>
       <c r="D131" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E131">
         <v>2015</v>
@@ -6125,16 +6203,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B132" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C132" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D132" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E132">
         <v>2015</v>
@@ -6142,16 +6220,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B133" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C133" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D133" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E133">
         <v>2015</v>
@@ -6159,16 +6237,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>325</v>
+      </c>
+      <c r="B134" t="s">
+        <v>326</v>
+      </c>
+      <c r="C134" t="s">
         <v>327</v>
       </c>
-      <c r="B134" t="s">
-        <v>328</v>
-      </c>
-      <c r="C134" t="s">
-        <v>329</v>
-      </c>
       <c r="D134" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E134">
         <v>2015</v>
@@ -6176,16 +6254,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>328</v>
+      </c>
+      <c r="B135" t="s">
+        <v>329</v>
+      </c>
+      <c r="C135" t="s">
         <v>330</v>
       </c>
-      <c r="B135" t="s">
-        <v>331</v>
-      </c>
-      <c r="C135" t="s">
-        <v>332</v>
-      </c>
       <c r="D135" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E135">
         <v>2015</v>
@@ -6193,16 +6271,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B136" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C136" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D136" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E136">
         <v>2015</v>
@@ -6210,16 +6288,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B137" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C137" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D137" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E137">
         <v>2015</v>
@@ -6227,16 +6305,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>335</v>
+      </c>
+      <c r="B138" t="s">
+        <v>336</v>
+      </c>
+      <c r="C138" t="s">
         <v>337</v>
       </c>
-      <c r="B138" t="s">
-        <v>338</v>
-      </c>
-      <c r="C138" t="s">
-        <v>339</v>
-      </c>
       <c r="D138" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E138">
         <v>2015</v>
@@ -6244,16 +6322,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B139" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C139" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D139" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E139">
         <v>2016</v>
@@ -6261,16 +6339,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B140" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C140" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D140" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E140">
         <v>2016</v>
@@ -6278,16 +6356,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B141" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C141" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D141" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E141">
         <v>2016</v>
@@ -6295,16 +6373,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B142" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C142" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D142" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E142">
         <v>2016</v>
@@ -6312,16 +6390,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B143" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C143" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D143" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E143">
         <v>2016</v>
@@ -6329,16 +6407,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B144" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C144" t="s">
         <v>101</v>
       </c>
       <c r="D144" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E144">
         <v>2016</v>
@@ -6346,16 +6424,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B145" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C145" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D145" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E145">
         <v>2016</v>
@@ -6363,16 +6441,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B146" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C146" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D146" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E146">
         <v>2016</v>
@@ -6380,16 +6458,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B147" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C147" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D147" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E147">
         <v>2016</v>
@@ -6397,16 +6475,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B148" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C148" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D148" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E148">
         <v>2016</v>
@@ -6414,16 +6492,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B149" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C149" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D149" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E149">
         <v>2016</v>
@@ -6431,16 +6509,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B150" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C150" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D150" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E150">
         <v>2016</v>
@@ -6448,16 +6526,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B151" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C151" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D151" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E151">
         <v>2016</v>
@@ -6465,16 +6543,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B152" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C152" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D152" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E152">
         <v>2016</v>
@@ -6482,16 +6560,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B153" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C153" t="s">
         <v>26</v>
       </c>
       <c r="D153" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E153">
         <v>2016</v>
@@ -6499,16 +6577,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B154" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C154" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D154" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E154">
         <v>2017</v>
@@ -6516,16 +6594,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B155" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C155" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D155" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E155">
         <v>2017</v>
@@ -6533,16 +6611,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B156" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C156" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D156" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E156">
         <v>2017</v>
@@ -6550,16 +6628,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B157" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C157" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D157" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E157">
         <v>2017</v>
@@ -6567,16 +6645,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B158" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C158" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D158" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E158">
         <v>2017</v>
@@ -6584,16 +6662,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B159" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C159" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D159" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E159">
         <v>2017</v>
@@ -6601,16 +6679,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B160" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C160" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D160" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E160">
         <v>2017</v>
@@ -6618,16 +6696,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B161" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C161" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D161" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E161">
         <v>2017</v>
@@ -6635,16 +6713,16 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B162" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C162" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D162" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E162">
         <v>2017</v>
@@ -6652,16 +6730,16 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B163" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C163" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D163" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E163">
         <v>2017</v>
@@ -6669,16 +6747,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B164" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C164" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D164" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E164">
         <v>2017</v>
@@ -6686,16 +6764,16 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B165" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C165" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D165" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E165">
         <v>2017</v>
@@ -6703,16 +6781,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B166" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C166" t="s">
         <v>101</v>
       </c>
       <c r="D166" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E166">
         <v>2017</v>
@@ -6720,16 +6798,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>388</v>
+      </c>
+      <c r="B167" t="s">
         <v>390</v>
       </c>
-      <c r="B167" t="s">
-        <v>392</v>
-      </c>
       <c r="C167" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D167" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E167">
         <v>2017</v>
@@ -6737,16 +6815,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B168" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C168" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D168" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E168">
         <v>2018</v>
@@ -6754,16 +6832,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B169" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C169" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D169" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E169">
         <v>2018</v>
@@ -6771,16 +6849,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B170" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C170" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D170" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E170">
         <v>2018</v>
@@ -6788,16 +6866,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B171" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C171" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D171" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E171">
         <v>2018</v>
@@ -6805,16 +6883,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B172" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C172" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D172" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E172">
         <v>2018</v>
@@ -6822,16 +6900,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B173" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C173" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D173" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E173">
         <v>2018</v>
@@ -6839,16 +6917,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B174" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C174" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D174" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E174">
         <v>2018</v>
@@ -6856,16 +6934,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B175" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C175" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D175" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E175">
         <v>2018</v>
@@ -6873,16 +6951,16 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B176" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C176" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D176" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E176">
         <v>2018</v>
@@ -6890,16 +6968,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B177" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C177" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D177" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E177">
         <v>2018</v>
@@ -6907,16 +6985,16 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B178" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C178" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D178" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E178">
         <v>2018</v>
@@ -6924,16 +7002,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B179" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C179" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D179" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E179">
         <v>2018</v>
@@ -6941,16 +7019,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B180" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C180" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D180" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E180">
         <v>2018</v>
@@ -6958,16 +7036,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B181" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C181" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D181" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E181">
         <v>2018</v>
@@ -6975,16 +7053,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B182" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C182" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D182" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E182">
         <v>2018</v>
@@ -6992,16 +7070,16 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B183" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C183" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D183" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E183">
         <v>2018</v>
@@ -7009,16 +7087,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B184" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C184" t="s">
         <v>13</v>
       </c>
       <c r="D184" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E184">
         <v>2018</v>
@@ -7026,16 +7104,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B185" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C185" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D185" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E185">
         <v>2018</v>
@@ -7043,16 +7121,16 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B186" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C186" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D186" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E186">
         <v>2018</v>
@@ -7060,16 +7138,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B187" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C187" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D187" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E187">
         <v>2018</v>
@@ -7077,16 +7155,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B188" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C188" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D188" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E188">
         <v>2018</v>
@@ -7094,16 +7172,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B189" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C189" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D189" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E189">
         <v>2018</v>
@@ -7111,16 +7189,16 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B190" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C190" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D190" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E190">
         <v>2018</v>
@@ -7128,16 +7206,16 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B191" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C191" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D191" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E191">
         <v>2018</v>
@@ -7145,16 +7223,16 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B192" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C192" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D192" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E192">
         <v>2019</v>
@@ -7162,16 +7240,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B193" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C193" t="s">
         <v>26</v>
       </c>
       <c r="D193" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E193">
         <v>2019</v>
@@ -7179,16 +7257,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B194" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C194" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D194" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E194">
         <v>2019</v>
@@ -7196,16 +7274,16 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B195" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C195" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D195" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E195">
         <v>2019</v>
@@ -7213,16 +7291,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B196" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C196" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D196" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E196">
         <v>2019</v>
@@ -7230,16 +7308,16 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B197" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C197" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D197" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E197">
         <v>2019</v>
@@ -7247,16 +7325,16 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B198" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C198" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D198" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E198">
         <v>2019</v>
@@ -7264,16 +7342,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B199" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C199" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D199" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E199">
         <v>2019</v>
@@ -7281,16 +7359,16 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B200" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C200" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E200">
         <v>2019</v>
@@ -7298,16 +7376,16 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B201" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C201" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D201" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E201">
         <v>2019</v>
@@ -7315,16 +7393,16 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B202" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C202" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D202" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E202">
         <v>2019</v>
@@ -7332,16 +7410,16 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B203" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C203" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D203" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E203">
         <v>2020</v>
@@ -7349,16 +7427,16 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B204" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C204" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D204" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E204">
         <v>2020</v>
@@ -7366,16 +7444,16 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B205" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C205" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D205" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E205">
         <v>2020</v>
@@ -7383,16 +7461,16 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B206" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C206" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D206" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E206">
         <v>2020</v>
@@ -7400,16 +7478,16 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B207" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C207" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D207" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E207">
         <v>2020</v>
@@ -7417,16 +7495,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B208" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C208" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D208" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E208">
         <v>2020</v>
@@ -7434,16 +7512,16 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B209" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C209" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D209" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E209">
         <v>2020</v>
@@ -7451,16 +7529,16 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B210" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C210" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D210" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E210">
         <v>2020</v>
@@ -7468,16 +7546,16 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B211" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C211" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D211" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E211">
         <v>2021</v>
@@ -7485,16 +7563,16 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B212" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C212" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D212" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E212">
         <v>2021</v>
@@ -7502,16 +7580,16 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B213" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C213" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D213" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E213">
         <v>2021</v>
@@ -7519,16 +7597,16 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B214" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C214" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D214" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E214">
         <v>2021</v>
@@ -7536,16 +7614,16 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B215" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C215" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D215" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E215">
         <v>2021</v>
@@ -7553,16 +7631,16 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B216" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C216" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D216" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E216">
         <v>2021</v>
@@ -7570,16 +7648,16 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B217" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C217" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D217" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E217">
         <v>2021</v>
@@ -7587,16 +7665,16 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B218" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C218" t="s">
         <v>101</v>
       </c>
       <c r="D218" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E218">
         <v>2021</v>
@@ -7604,16 +7682,16 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B219" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C219" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D219" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E219">
         <v>2021</v>
@@ -7621,16 +7699,16 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B220" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C220" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D220" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E220">
         <v>2021</v>
@@ -7638,19 +7716,206 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B221" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C221" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D221" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E221">
         <v>2021</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>561</v>
+      </c>
+      <c r="B222" t="s">
+        <v>574</v>
+      </c>
+      <c r="C222" t="s">
+        <v>573</v>
+      </c>
+      <c r="D222" t="s">
+        <v>255</v>
+      </c>
+      <c r="E222">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>562</v>
+      </c>
+      <c r="B223" t="s">
+        <v>575</v>
+      </c>
+      <c r="C223" t="s">
+        <v>538</v>
+      </c>
+      <c r="D223" t="s">
+        <v>255</v>
+      </c>
+      <c r="E223">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>563</v>
+      </c>
+      <c r="B224" t="s">
+        <v>572</v>
+      </c>
+      <c r="C224" t="s">
+        <v>576</v>
+      </c>
+      <c r="D224" t="s">
+        <v>255</v>
+      </c>
+      <c r="E224">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>564</v>
+      </c>
+      <c r="B225" t="s">
+        <v>577</v>
+      </c>
+      <c r="C225" t="s">
+        <v>578</v>
+      </c>
+      <c r="D225" t="s">
+        <v>255</v>
+      </c>
+      <c r="E225">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>565</v>
+      </c>
+      <c r="B226" t="s">
+        <v>579</v>
+      </c>
+      <c r="C226" t="s">
+        <v>580</v>
+      </c>
+      <c r="D226" t="s">
+        <v>255</v>
+      </c>
+      <c r="E226">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>566</v>
+      </c>
+      <c r="B227" t="s">
+        <v>581</v>
+      </c>
+      <c r="C227" t="s">
+        <v>327</v>
+      </c>
+      <c r="D227" t="s">
+        <v>255</v>
+      </c>
+      <c r="E227">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>567</v>
+      </c>
+      <c r="B228" t="s">
+        <v>582</v>
+      </c>
+      <c r="C228" t="s">
+        <v>146</v>
+      </c>
+      <c r="D228" t="s">
+        <v>255</v>
+      </c>
+      <c r="E228">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>568</v>
+      </c>
+      <c r="B229" t="s">
+        <v>583</v>
+      </c>
+      <c r="C229" t="s">
+        <v>291</v>
+      </c>
+      <c r="D229" t="s">
+        <v>255</v>
+      </c>
+      <c r="E229">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>569</v>
+      </c>
+      <c r="B230" t="s">
+        <v>584</v>
+      </c>
+      <c r="C230" t="s">
+        <v>585</v>
+      </c>
+      <c r="D230" t="s">
+        <v>255</v>
+      </c>
+      <c r="E230">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>570</v>
+      </c>
+      <c r="B231" t="s">
+        <v>586</v>
+      </c>
+      <c r="C231" t="s">
+        <v>327</v>
+      </c>
+      <c r="D231" t="s">
+        <v>255</v>
+      </c>
+      <c r="E231">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>571</v>
+      </c>
+      <c r="B232" t="s">
+        <v>587</v>
+      </c>
+      <c r="C232" t="s">
+        <v>467</v>
+      </c>
+      <c r="D232" t="s">
+        <v>255</v>
+      </c>
+      <c r="E232">
+        <v>2022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>